<commit_message>
Added functions to automatically format Class 1
</commit_message>
<xml_diff>
--- a/Data/2001 STOP Summary.xlsx
+++ b/Data/2001 STOP Summary.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="390" yWindow="0" windowWidth="28320" windowHeight="15600" tabRatio="652" firstSheet="1" activeTab="7" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="390" yWindow="0" windowWidth="28320" windowHeight="15600" tabRatio="652" firstSheet="3" activeTab="7" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet name="SummaryStats" sheetId="1" state="visible" r:id="rId1"/>
@@ -554,14 +554,14 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="18" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="18" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="5" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -1978,7 +1978,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:O199"/>
+  <dimension ref="A1:P199"/>
   <sheetViews>
     <sheetView topLeftCell="A8" workbookViewId="0">
       <selection activeCell="A46" sqref="A46"/>
@@ -1989,13 +1989,13 @@
     <col width="5.140625" customWidth="1" style="15" min="1" max="1"/>
     <col width="33" bestFit="1" customWidth="1" style="15" min="2" max="2"/>
     <col width="10.28515625" customWidth="1" style="15" min="3" max="15"/>
-    <col width="9.140625" customWidth="1" style="15" min="16" max="17"/>
-    <col width="9.140625" customWidth="1" style="15" min="18" max="16384"/>
+    <col width="9.140625" customWidth="1" style="15" min="16" max="18"/>
+    <col width="9.140625" customWidth="1" style="15" min="19" max="16384"/>
   </cols>
   <sheetData>
     <row r="1">
       <c r="A1" s="81" t="n"/>
-      <c r="B1" s="78" t="n"/>
+      <c r="B1" s="76" t="n"/>
       <c r="C1" s="1" t="n"/>
       <c r="D1" s="1" t="n"/>
       <c r="E1" s="1" t="n"/>
@@ -2013,67 +2013,67 @@
     <row r="2" ht="12.75" customHeight="1">
       <c r="A2" s="82" t="n"/>
       <c r="B2" s="83" t="n"/>
-      <c r="C2" s="75" t="inlineStr">
+      <c r="C2" s="79" t="inlineStr">
         <is>
           <t>10-A DAA, Tulelake-Butte Valley Fair</t>
         </is>
       </c>
-      <c r="D2" s="75" t="inlineStr">
+      <c r="D2" s="79" t="inlineStr">
         <is>
           <t>33rd DAA, San Benito County Fair</t>
         </is>
       </c>
-      <c r="E2" s="75" t="inlineStr">
+      <c r="E2" s="79" t="inlineStr">
         <is>
           <t>34th DAA, Modoc-Last Frontier Fair</t>
         </is>
       </c>
-      <c r="F2" s="75" t="inlineStr">
+      <c r="F2" s="79" t="inlineStr">
         <is>
           <t>41st DAA, Del Norte County Fair</t>
         </is>
       </c>
-      <c r="G2" s="75" t="inlineStr">
+      <c r="G2" s="79" t="inlineStr">
         <is>
           <t>44th DAA, Colusa County Fair</t>
         </is>
       </c>
-      <c r="H2" s="75" t="inlineStr">
+      <c r="H2" s="79" t="inlineStr">
         <is>
           <t>51st DAA, San Fernando Valley Fair</t>
         </is>
       </c>
-      <c r="I2" s="75" t="inlineStr">
+      <c r="I2" s="79" t="inlineStr">
         <is>
           <t>52nd DAA, Sacto. County Fair</t>
         </is>
       </c>
-      <c r="J2" s="75" t="inlineStr">
+      <c r="J2" s="79" t="inlineStr">
         <is>
           <t>54th DAA, Colorado River Country</t>
         </is>
       </c>
-      <c r="K2" s="75" t="inlineStr">
+      <c r="K2" s="79" t="inlineStr">
         <is>
           <t>Cloverdale Citrus Fair</t>
         </is>
       </c>
-      <c r="L2" s="75" t="inlineStr">
+      <c r="L2" s="79" t="inlineStr">
         <is>
           <t>Chowchilla- Madera County Fair</t>
         </is>
       </c>
-      <c r="M2" s="75" t="inlineStr">
+      <c r="M2" s="79" t="inlineStr">
         <is>
           <t>Mendocino County Fair</t>
         </is>
       </c>
-      <c r="N2" s="75" t="inlineStr">
+      <c r="N2" s="79" t="inlineStr">
         <is>
           <t>Inter-Mountain Fair of Shasta</t>
         </is>
       </c>
-      <c r="O2" s="75" t="inlineStr">
+      <c r="O2" s="79" t="inlineStr">
         <is>
           <t>Trinity County Fair</t>
         </is>
@@ -2082,23 +2082,23 @@
     <row r="3" ht="49.5" customHeight="1">
       <c r="A3" s="82" t="n"/>
       <c r="B3" s="83" t="n"/>
-      <c r="C3" s="76" t="n"/>
-      <c r="D3" s="76" t="n"/>
-      <c r="E3" s="76" t="n"/>
-      <c r="F3" s="76" t="n"/>
-      <c r="G3" s="76" t="n"/>
-      <c r="H3" s="76" t="n"/>
-      <c r="I3" s="76" t="n"/>
-      <c r="J3" s="76" t="n"/>
-      <c r="K3" s="76" t="n"/>
-      <c r="L3" s="76" t="n"/>
-      <c r="M3" s="76" t="n"/>
-      <c r="N3" s="76" t="n"/>
-      <c r="O3" s="76" t="n"/>
+      <c r="C3" s="80" t="n"/>
+      <c r="D3" s="80" t="n"/>
+      <c r="E3" s="80" t="n"/>
+      <c r="F3" s="80" t="n"/>
+      <c r="G3" s="80" t="n"/>
+      <c r="H3" s="80" t="n"/>
+      <c r="I3" s="80" t="n"/>
+      <c r="J3" s="80" t="n"/>
+      <c r="K3" s="80" t="n"/>
+      <c r="L3" s="80" t="n"/>
+      <c r="M3" s="80" t="n"/>
+      <c r="N3" s="80" t="n"/>
+      <c r="O3" s="80" t="n"/>
     </row>
     <row r="4" hidden="1" ht="3.75" customHeight="1">
-      <c r="A4" s="79" t="n"/>
-      <c r="B4" s="80" t="n"/>
+      <c r="A4" s="77" t="n"/>
+      <c r="B4" s="78" t="n"/>
       <c r="C4" s="2" t="n"/>
       <c r="D4" s="2" t="n"/>
       <c r="E4" s="2" t="n"/>
@@ -3893,8 +3893,8 @@
       <c r="O47" s="19" t="n"/>
     </row>
     <row r="48" ht="9.75" customHeight="1">
-      <c r="A48" s="77" t="n"/>
-      <c r="B48" s="78" t="n"/>
+      <c r="A48" s="75" t="n"/>
+      <c r="B48" s="76" t="n"/>
       <c r="C48" s="1" t="n"/>
       <c r="D48" s="1" t="n"/>
       <c r="E48" s="1" t="n"/>
@@ -3910,8 +3910,8 @@
       <c r="O48" s="1" t="n"/>
     </row>
     <row r="49" ht="64.5" customHeight="1">
-      <c r="A49" s="79" t="n"/>
-      <c r="B49" s="80" t="n"/>
+      <c r="A49" s="77" t="n"/>
+      <c r="B49" s="78" t="n"/>
       <c r="C49" s="16" t="inlineStr">
         <is>
           <t>10-A DAA, Tulelake-Butte Valley Fair</t>
@@ -3985,14 +3985,14 @@
         </is>
       </c>
       <c r="B50" s="6" t="n"/>
-      <c r="C50" s="77" t="n"/>
-      <c r="D50" s="77" t="n"/>
-      <c r="E50" s="77" t="n"/>
-      <c r="F50" s="77" t="n"/>
-      <c r="G50" s="77" t="n"/>
-      <c r="H50" s="77" t="n"/>
-      <c r="I50" s="77" t="n"/>
-      <c r="J50" s="77" t="n"/>
+      <c r="C50" s="75" t="n"/>
+      <c r="D50" s="75" t="n"/>
+      <c r="E50" s="75" t="n"/>
+      <c r="F50" s="75" t="n"/>
+      <c r="G50" s="75" t="n"/>
+      <c r="H50" s="75" t="n"/>
+      <c r="I50" s="75" t="n"/>
+      <c r="J50" s="75" t="n"/>
       <c r="K50" s="23" t="n"/>
       <c r="L50" s="23" t="n"/>
       <c r="M50" s="23" t="n"/>
@@ -4006,19 +4006,19 @@
         </is>
       </c>
       <c r="B51" s="6" t="n"/>
-      <c r="C51" s="77" t="n"/>
-      <c r="D51" s="77" t="n"/>
-      <c r="E51" s="77" t="n"/>
-      <c r="F51" s="77" t="n"/>
-      <c r="G51" s="77" t="n"/>
-      <c r="H51" s="77" t="n"/>
-      <c r="I51" s="77" t="n"/>
-      <c r="J51" s="77" t="n"/>
-      <c r="K51" s="77" t="n"/>
-      <c r="L51" s="77" t="n"/>
-      <c r="M51" s="77" t="n"/>
-      <c r="N51" s="77" t="n"/>
-      <c r="O51" s="77" t="n"/>
+      <c r="C51" s="75" t="n"/>
+      <c r="D51" s="75" t="n"/>
+      <c r="E51" s="75" t="n"/>
+      <c r="F51" s="75" t="n"/>
+      <c r="G51" s="75" t="n"/>
+      <c r="H51" s="75" t="n"/>
+      <c r="I51" s="75" t="n"/>
+      <c r="J51" s="75" t="n"/>
+      <c r="K51" s="75" t="n"/>
+      <c r="L51" s="75" t="n"/>
+      <c r="M51" s="75" t="n"/>
+      <c r="N51" s="75" t="n"/>
+      <c r="O51" s="75" t="n"/>
     </row>
     <row r="52">
       <c r="A52" s="5" t="n"/>
@@ -4445,18 +4445,18 @@
         </is>
       </c>
       <c r="B62" s="6" t="n"/>
-      <c r="C62" s="77" t="n"/>
-      <c r="D62" s="77" t="n"/>
-      <c r="E62" s="77" t="n"/>
-      <c r="F62" s="77" t="n"/>
-      <c r="G62" s="77" t="n"/>
-      <c r="I62" s="77" t="n"/>
-      <c r="J62" s="77" t="n"/>
-      <c r="K62" s="77" t="n"/>
-      <c r="L62" s="77" t="n"/>
-      <c r="M62" s="77" t="n"/>
-      <c r="N62" s="77" t="n"/>
-      <c r="O62" s="77" t="n"/>
+      <c r="C62" s="75" t="n"/>
+      <c r="D62" s="75" t="n"/>
+      <c r="E62" s="75" t="n"/>
+      <c r="F62" s="75" t="n"/>
+      <c r="G62" s="75" t="n"/>
+      <c r="I62" s="75" t="n"/>
+      <c r="J62" s="75" t="n"/>
+      <c r="K62" s="75" t="n"/>
+      <c r="L62" s="75" t="n"/>
+      <c r="M62" s="75" t="n"/>
+      <c r="N62" s="75" t="n"/>
+      <c r="O62" s="75" t="n"/>
     </row>
     <row r="63">
       <c r="A63" s="5" t="n"/>
@@ -4813,19 +4813,19 @@
         </is>
       </c>
       <c r="B71" s="6" t="n"/>
-      <c r="C71" s="77" t="n"/>
-      <c r="D71" s="77" t="n"/>
-      <c r="E71" s="77" t="n"/>
-      <c r="F71" s="77" t="n"/>
-      <c r="G71" s="77" t="n"/>
+      <c r="C71" s="75" t="n"/>
+      <c r="D71" s="75" t="n"/>
+      <c r="E71" s="75" t="n"/>
+      <c r="F71" s="75" t="n"/>
+      <c r="G71" s="75" t="n"/>
       <c r="H71" s="7" t="n"/>
-      <c r="I71" s="77" t="n"/>
-      <c r="J71" s="77" t="n"/>
-      <c r="K71" s="77" t="n"/>
-      <c r="L71" s="77" t="n"/>
-      <c r="M71" s="77" t="n"/>
-      <c r="N71" s="77" t="n"/>
-      <c r="O71" s="77" t="n"/>
+      <c r="I71" s="75" t="n"/>
+      <c r="J71" s="75" t="n"/>
+      <c r="K71" s="75" t="n"/>
+      <c r="L71" s="75" t="n"/>
+      <c r="M71" s="75" t="n"/>
+      <c r="N71" s="75" t="n"/>
+      <c r="O71" s="75" t="n"/>
     </row>
     <row r="72">
       <c r="A72" s="5" t="n"/>
@@ -5209,6 +5209,11 @@
     <row r="199"/>
   </sheetData>
   <mergeCells count="15">
+    <mergeCell ref="N2:N3"/>
+    <mergeCell ref="O2:O3"/>
+    <mergeCell ref="K2:K3"/>
+    <mergeCell ref="L2:L3"/>
+    <mergeCell ref="M2:M3"/>
     <mergeCell ref="A48:B49"/>
     <mergeCell ref="J2:J3"/>
     <mergeCell ref="F2:F3"/>
@@ -5219,11 +5224,6 @@
     <mergeCell ref="D2:D3"/>
     <mergeCell ref="A1:B4"/>
     <mergeCell ref="E2:E3"/>
-    <mergeCell ref="N2:N3"/>
-    <mergeCell ref="O2:O3"/>
-    <mergeCell ref="K2:K3"/>
-    <mergeCell ref="L2:L3"/>
-    <mergeCell ref="M2:M3"/>
   </mergeCells>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.5" right="0.5" top="0.5" bottom="0.5" header="0.25" footer="0.25"/>
@@ -5260,13 +5260,13 @@
     <col width="5.140625" customWidth="1" style="15" min="1" max="1"/>
     <col width="33" bestFit="1" customWidth="1" style="15" min="2" max="2"/>
     <col width="10.28515625" customWidth="1" style="15" min="3" max="22"/>
-    <col width="9.140625" customWidth="1" style="15" min="23" max="24"/>
-    <col width="9.140625" customWidth="1" style="15" min="25" max="16384"/>
+    <col width="9.140625" customWidth="1" style="15" min="23" max="25"/>
+    <col width="9.140625" customWidth="1" style="15" min="26" max="16384"/>
   </cols>
   <sheetData>
     <row r="1">
       <c r="A1" s="81" t="n"/>
-      <c r="B1" s="78" t="n"/>
+      <c r="B1" s="76" t="n"/>
       <c r="C1" s="1" t="n"/>
       <c r="D1" s="1" t="n"/>
       <c r="E1" s="1" t="n"/>
@@ -5291,102 +5291,102 @@
     <row r="2">
       <c r="A2" s="82" t="n"/>
       <c r="B2" s="83" t="n"/>
-      <c r="C2" s="75" t="inlineStr">
+      <c r="C2" s="79" t="inlineStr">
         <is>
           <t>10th DAA, Siskiyou Golden Fair</t>
         </is>
       </c>
-      <c r="D2" s="75" t="inlineStr">
+      <c r="D2" s="79" t="inlineStr">
         <is>
           <t>12th DAA, Redwood Empire Fair</t>
         </is>
       </c>
-      <c r="E2" s="75" t="inlineStr">
+      <c r="E2" s="79" t="inlineStr">
         <is>
           <t>18th DAA, Eastern Sierra Tri-County Fair</t>
         </is>
       </c>
-      <c r="F2" s="75" t="inlineStr">
+      <c r="F2" s="79" t="inlineStr">
         <is>
           <t>20th DAA, Gold Country Fair</t>
         </is>
       </c>
-      <c r="G2" s="75" t="inlineStr">
+      <c r="G2" s="79" t="inlineStr">
         <is>
           <t>24-A DAA, Kings Fair</t>
         </is>
       </c>
-      <c r="H2" s="75" t="inlineStr">
+      <c r="H2" s="79" t="inlineStr">
         <is>
           <t>26th DAA, Amador County Fair</t>
         </is>
       </c>
-      <c r="I2" s="75" t="inlineStr">
+      <c r="I2" s="79" t="inlineStr">
         <is>
           <t>29th DAA, Mother Lode Fair</t>
         </is>
       </c>
-      <c r="J2" s="75" t="inlineStr">
+      <c r="J2" s="79" t="inlineStr">
         <is>
           <t>30th DAA, Tehama District Fair</t>
         </is>
       </c>
-      <c r="K2" s="75" t="inlineStr">
+      <c r="K2" s="79" t="inlineStr">
         <is>
           <t>35-A DAA, Mariposa County Fair</t>
         </is>
       </c>
-      <c r="L2" s="75" t="inlineStr">
+      <c r="L2" s="79" t="inlineStr">
         <is>
           <t>36th DAA, Dixon May Fair</t>
         </is>
       </c>
-      <c r="M2" s="75" t="inlineStr">
+      <c r="M2" s="79" t="inlineStr">
         <is>
           <t>39th DAA, Calaveras County Fair</t>
         </is>
       </c>
-      <c r="N2" s="75" t="inlineStr">
+      <c r="N2" s="79" t="inlineStr">
         <is>
           <t>40th DAA, Yolo County Fair</t>
         </is>
       </c>
-      <c r="O2" s="75" t="inlineStr">
+      <c r="O2" s="79" t="inlineStr">
         <is>
           <t>42nd DAA, Glenn County Fair</t>
         </is>
       </c>
-      <c r="P2" s="75" t="inlineStr">
+      <c r="P2" s="79" t="inlineStr">
         <is>
           <t>48th DAA, Schools Involvement Fair</t>
         </is>
       </c>
-      <c r="Q2" s="75" t="inlineStr">
+      <c r="Q2" s="79" t="inlineStr">
         <is>
           <t>49th DAA, Lake County Fair</t>
         </is>
       </c>
-      <c r="R2" s="75" t="inlineStr">
+      <c r="R2" s="79" t="inlineStr">
         <is>
           <t>53rd DAA, Desert Empire Fair</t>
         </is>
       </c>
-      <c r="S2" s="75" t="inlineStr">
+      <c r="S2" s="79" t="inlineStr">
         <is>
           <t>Butte County Fair</t>
         </is>
       </c>
-      <c r="T2" s="75" t="inlineStr">
+      <c r="T2" s="79" t="inlineStr">
         <is>
           <t>Lassen County Fair</t>
         </is>
       </c>
-      <c r="U2" s="75" t="inlineStr">
+      <c r="U2" s="79" t="inlineStr">
         <is>
           <t>Merced County Fair</t>
         </is>
       </c>
-      <c r="V2" s="75" t="inlineStr">
+      <c r="V2" s="79" t="inlineStr">
         <is>
           <t>Plumas Sierra County Fair (1/01 - 6/01)</t>
         </is>
@@ -5395,30 +5395,30 @@
     <row r="3" ht="48.95" customHeight="1">
       <c r="A3" s="82" t="n"/>
       <c r="B3" s="83" t="n"/>
-      <c r="C3" s="76" t="n"/>
-      <c r="D3" s="76" t="n"/>
-      <c r="E3" s="76" t="n"/>
-      <c r="F3" s="76" t="n"/>
-      <c r="G3" s="76" t="n"/>
-      <c r="H3" s="76" t="n"/>
-      <c r="I3" s="76" t="n"/>
-      <c r="J3" s="76" t="n"/>
-      <c r="K3" s="76" t="n"/>
-      <c r="L3" s="76" t="n"/>
-      <c r="M3" s="76" t="n"/>
-      <c r="N3" s="76" t="n"/>
-      <c r="O3" s="76" t="n"/>
-      <c r="P3" s="76" t="n"/>
-      <c r="Q3" s="76" t="n"/>
-      <c r="R3" s="76" t="n"/>
-      <c r="S3" s="76" t="n"/>
-      <c r="T3" s="76" t="n"/>
-      <c r="U3" s="76" t="n"/>
-      <c r="V3" s="76" t="n"/>
+      <c r="C3" s="80" t="n"/>
+      <c r="D3" s="80" t="n"/>
+      <c r="E3" s="80" t="n"/>
+      <c r="F3" s="80" t="n"/>
+      <c r="G3" s="80" t="n"/>
+      <c r="H3" s="80" t="n"/>
+      <c r="I3" s="80" t="n"/>
+      <c r="J3" s="80" t="n"/>
+      <c r="K3" s="80" t="n"/>
+      <c r="L3" s="80" t="n"/>
+      <c r="M3" s="80" t="n"/>
+      <c r="N3" s="80" t="n"/>
+      <c r="O3" s="80" t="n"/>
+      <c r="P3" s="80" t="n"/>
+      <c r="Q3" s="80" t="n"/>
+      <c r="R3" s="80" t="n"/>
+      <c r="S3" s="80" t="n"/>
+      <c r="T3" s="80" t="n"/>
+      <c r="U3" s="80" t="n"/>
+      <c r="V3" s="80" t="n"/>
     </row>
     <row r="4" ht="5.1" customHeight="1">
-      <c r="A4" s="79" t="n"/>
-      <c r="B4" s="80" t="n"/>
+      <c r="A4" s="77" t="n"/>
+      <c r="B4" s="78" t="n"/>
       <c r="C4" s="2" t="n"/>
       <c r="D4" s="2" t="n"/>
       <c r="E4" s="2" t="n"/>
@@ -7999,8 +7999,8 @@
       <c r="V47" s="36" t="n"/>
     </row>
     <row r="48" ht="10.5" customHeight="1">
-      <c r="A48" s="77" t="n"/>
-      <c r="B48" s="78" t="n"/>
+      <c r="A48" s="75" t="n"/>
+      <c r="B48" s="76" t="n"/>
       <c r="C48" s="1" t="n"/>
       <c r="D48" s="1" t="n"/>
       <c r="E48" s="1" t="n"/>
@@ -8023,8 +8023,8 @@
       <c r="V48" s="1" t="n"/>
     </row>
     <row r="49" ht="76.5" customHeight="1">
-      <c r="A49" s="79" t="n"/>
-      <c r="B49" s="80" t="n"/>
+      <c r="A49" s="77" t="n"/>
+      <c r="B49" s="78" t="n"/>
       <c r="C49" s="16" t="inlineStr">
         <is>
           <t>10th DAA, Siskiyou Golden Fair</t>
@@ -8133,26 +8133,26 @@
         </is>
       </c>
       <c r="B50" s="6" t="n"/>
-      <c r="C50" s="77" t="n"/>
-      <c r="D50" s="77" t="n"/>
-      <c r="E50" s="77" t="n"/>
-      <c r="F50" s="77" t="n"/>
-      <c r="G50" s="77" t="n"/>
-      <c r="H50" s="77" t="n"/>
-      <c r="I50" s="77" t="n"/>
-      <c r="J50" s="77" t="n"/>
-      <c r="K50" s="77" t="n"/>
-      <c r="L50" s="77" t="n"/>
-      <c r="M50" s="77" t="n"/>
-      <c r="N50" s="77" t="n"/>
-      <c r="O50" s="77" t="n"/>
-      <c r="P50" s="77" t="n"/>
-      <c r="Q50" s="77" t="n"/>
-      <c r="R50" s="77" t="n"/>
-      <c r="S50" s="77" t="n"/>
-      <c r="T50" s="77" t="n"/>
-      <c r="U50" s="77" t="n"/>
-      <c r="V50" s="77" t="n"/>
+      <c r="C50" s="75" t="n"/>
+      <c r="D50" s="75" t="n"/>
+      <c r="E50" s="75" t="n"/>
+      <c r="F50" s="75" t="n"/>
+      <c r="G50" s="75" t="n"/>
+      <c r="H50" s="75" t="n"/>
+      <c r="I50" s="75" t="n"/>
+      <c r="J50" s="75" t="n"/>
+      <c r="K50" s="75" t="n"/>
+      <c r="L50" s="75" t="n"/>
+      <c r="M50" s="75" t="n"/>
+      <c r="N50" s="75" t="n"/>
+      <c r="O50" s="75" t="n"/>
+      <c r="P50" s="75" t="n"/>
+      <c r="Q50" s="75" t="n"/>
+      <c r="R50" s="75" t="n"/>
+      <c r="S50" s="75" t="n"/>
+      <c r="T50" s="75" t="n"/>
+      <c r="U50" s="75" t="n"/>
+      <c r="V50" s="75" t="n"/>
     </row>
     <row r="51">
       <c r="A51" s="3" t="inlineStr">
@@ -8161,26 +8161,26 @@
         </is>
       </c>
       <c r="B51" s="6" t="n"/>
-      <c r="C51" s="77" t="n"/>
-      <c r="D51" s="77" t="n"/>
-      <c r="E51" s="77" t="n"/>
-      <c r="F51" s="77" t="n"/>
-      <c r="G51" s="77" t="n"/>
-      <c r="H51" s="77" t="n"/>
-      <c r="I51" s="77" t="n"/>
-      <c r="J51" s="77" t="n"/>
-      <c r="K51" s="77" t="n"/>
-      <c r="L51" s="77" t="n"/>
-      <c r="M51" s="77" t="n"/>
-      <c r="N51" s="77" t="n"/>
-      <c r="O51" s="77" t="n"/>
-      <c r="P51" s="77" t="n"/>
-      <c r="Q51" s="77" t="n"/>
-      <c r="R51" s="77" t="n"/>
-      <c r="S51" s="77" t="n"/>
-      <c r="T51" s="77" t="n"/>
-      <c r="U51" s="77" t="n"/>
-      <c r="V51" s="77" t="n"/>
+      <c r="C51" s="75" t="n"/>
+      <c r="D51" s="75" t="n"/>
+      <c r="E51" s="75" t="n"/>
+      <c r="F51" s="75" t="n"/>
+      <c r="G51" s="75" t="n"/>
+      <c r="H51" s="75" t="n"/>
+      <c r="I51" s="75" t="n"/>
+      <c r="J51" s="75" t="n"/>
+      <c r="K51" s="75" t="n"/>
+      <c r="L51" s="75" t="n"/>
+      <c r="M51" s="75" t="n"/>
+      <c r="N51" s="75" t="n"/>
+      <c r="O51" s="75" t="n"/>
+      <c r="P51" s="75" t="n"/>
+      <c r="Q51" s="75" t="n"/>
+      <c r="R51" s="75" t="n"/>
+      <c r="S51" s="75" t="n"/>
+      <c r="T51" s="75" t="n"/>
+      <c r="U51" s="75" t="n"/>
+      <c r="V51" s="75" t="n"/>
     </row>
     <row r="52">
       <c r="A52" s="5" t="n"/>
@@ -8787,26 +8787,26 @@
         </is>
       </c>
       <c r="B62" s="6" t="n"/>
-      <c r="C62" s="77" t="n"/>
-      <c r="D62" s="77" t="n"/>
-      <c r="E62" s="77" t="n"/>
-      <c r="F62" s="77" t="n"/>
-      <c r="G62" s="77" t="n"/>
-      <c r="H62" s="77" t="n"/>
-      <c r="I62" s="77" t="n"/>
-      <c r="J62" s="77" t="n"/>
-      <c r="K62" s="77" t="n"/>
-      <c r="L62" s="77" t="n"/>
-      <c r="M62" s="77" t="n"/>
-      <c r="N62" s="77" t="n"/>
-      <c r="O62" s="77" t="n"/>
-      <c r="P62" s="77" t="n"/>
-      <c r="Q62" s="77" t="n"/>
-      <c r="R62" s="77" t="n"/>
-      <c r="S62" s="77" t="n"/>
-      <c r="T62" s="77" t="n"/>
-      <c r="U62" s="77" t="n"/>
-      <c r="V62" s="77" t="n"/>
+      <c r="C62" s="75" t="n"/>
+      <c r="D62" s="75" t="n"/>
+      <c r="E62" s="75" t="n"/>
+      <c r="F62" s="75" t="n"/>
+      <c r="G62" s="75" t="n"/>
+      <c r="H62" s="75" t="n"/>
+      <c r="I62" s="75" t="n"/>
+      <c r="J62" s="75" t="n"/>
+      <c r="K62" s="75" t="n"/>
+      <c r="L62" s="75" t="n"/>
+      <c r="M62" s="75" t="n"/>
+      <c r="N62" s="75" t="n"/>
+      <c r="O62" s="75" t="n"/>
+      <c r="P62" s="75" t="n"/>
+      <c r="Q62" s="75" t="n"/>
+      <c r="R62" s="75" t="n"/>
+      <c r="S62" s="75" t="n"/>
+      <c r="T62" s="75" t="n"/>
+      <c r="U62" s="75" t="n"/>
+      <c r="V62" s="75" t="n"/>
     </row>
     <row r="63">
       <c r="A63" s="5" t="n"/>
@@ -9319,26 +9319,26 @@
         </is>
       </c>
       <c r="B71" s="6" t="n"/>
-      <c r="C71" s="77" t="n"/>
-      <c r="D71" s="77" t="n"/>
-      <c r="E71" s="77" t="n"/>
-      <c r="F71" s="77" t="n"/>
-      <c r="G71" s="77" t="n"/>
-      <c r="H71" s="77" t="n"/>
-      <c r="I71" s="77" t="n"/>
-      <c r="J71" s="77" t="n"/>
-      <c r="K71" s="77" t="n"/>
-      <c r="L71" s="77" t="n"/>
-      <c r="M71" s="77" t="n"/>
-      <c r="N71" s="77" t="n"/>
-      <c r="O71" s="77" t="n"/>
-      <c r="P71" s="77" t="n"/>
-      <c r="Q71" s="77" t="n"/>
-      <c r="R71" s="77" t="n"/>
-      <c r="S71" s="77" t="n"/>
-      <c r="T71" s="77" t="n"/>
-      <c r="U71" s="77" t="n"/>
-      <c r="V71" s="77" t="n"/>
+      <c r="C71" s="75" t="n"/>
+      <c r="D71" s="75" t="n"/>
+      <c r="E71" s="75" t="n"/>
+      <c r="F71" s="75" t="n"/>
+      <c r="G71" s="75" t="n"/>
+      <c r="H71" s="75" t="n"/>
+      <c r="I71" s="75" t="n"/>
+      <c r="J71" s="75" t="n"/>
+      <c r="K71" s="75" t="n"/>
+      <c r="L71" s="75" t="n"/>
+      <c r="M71" s="75" t="n"/>
+      <c r="N71" s="75" t="n"/>
+      <c r="O71" s="75" t="n"/>
+      <c r="P71" s="75" t="n"/>
+      <c r="Q71" s="75" t="n"/>
+      <c r="R71" s="75" t="n"/>
+      <c r="S71" s="75" t="n"/>
+      <c r="T71" s="75" t="n"/>
+      <c r="U71" s="75" t="n"/>
+      <c r="V71" s="75" t="n"/>
     </row>
     <row r="72">
       <c r="A72" s="5" t="n"/>
@@ -9713,6 +9713,14 @@
     </row>
   </sheetData>
   <mergeCells count="22">
+    <mergeCell ref="S2:S3"/>
+    <mergeCell ref="T2:T3"/>
+    <mergeCell ref="U2:U3"/>
+    <mergeCell ref="V2:V3"/>
+    <mergeCell ref="O2:O3"/>
+    <mergeCell ref="P2:P3"/>
+    <mergeCell ref="Q2:Q3"/>
+    <mergeCell ref="R2:R3"/>
     <mergeCell ref="L2:L3"/>
     <mergeCell ref="M2:M3"/>
     <mergeCell ref="N2:N3"/>
@@ -9727,14 +9735,6 @@
     <mergeCell ref="D2:D3"/>
     <mergeCell ref="E2:E3"/>
     <mergeCell ref="K2:K3"/>
-    <mergeCell ref="S2:S3"/>
-    <mergeCell ref="T2:T3"/>
-    <mergeCell ref="U2:U3"/>
-    <mergeCell ref="V2:V3"/>
-    <mergeCell ref="O2:O3"/>
-    <mergeCell ref="P2:P3"/>
-    <mergeCell ref="Q2:Q3"/>
-    <mergeCell ref="R2:R3"/>
   </mergeCells>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.5" right="0.5" top="0.5" bottom="0.5" header="0.25" footer="0.25"/>
@@ -9771,13 +9771,13 @@
     <col width="5.140625" customWidth="1" style="15" min="1" max="1"/>
     <col width="33" bestFit="1" customWidth="1" style="15" min="2" max="2"/>
     <col width="10.28515625" customWidth="1" style="15" min="3" max="21"/>
-    <col width="9.140625" customWidth="1" style="15" min="22" max="23"/>
-    <col width="9.140625" customWidth="1" style="15" min="24" max="16384"/>
+    <col width="9.140625" customWidth="1" style="15" min="22" max="24"/>
+    <col width="9.140625" customWidth="1" style="15" min="25" max="16384"/>
   </cols>
   <sheetData>
     <row r="1" ht="11.25" customHeight="1">
       <c r="A1" s="81" t="n"/>
-      <c r="B1" s="78" t="n"/>
+      <c r="B1" s="76" t="n"/>
       <c r="C1" s="1" t="n"/>
       <c r="D1" s="1" t="n"/>
       <c r="E1" s="1" t="n"/>
@@ -9801,97 +9801,97 @@
     <row r="2">
       <c r="A2" s="82" t="n"/>
       <c r="B2" s="83" t="n"/>
-      <c r="C2" s="75" t="inlineStr">
+      <c r="C2" s="79" t="inlineStr">
         <is>
           <t>3rd DAA, Silver Dollar Fair</t>
         </is>
       </c>
-      <c r="D2" s="75" t="inlineStr">
+      <c r="D2" s="79" t="inlineStr">
         <is>
           <t>4th DAA, Sonoma Marin Fair</t>
         </is>
       </c>
-      <c r="E2" s="75" t="inlineStr">
+      <c r="E2" s="79" t="inlineStr">
         <is>
           <t>9th DAA, Redwood Acres Fair</t>
         </is>
       </c>
-      <c r="F2" s="75" t="inlineStr">
+      <c r="F2" s="79" t="inlineStr">
         <is>
           <t>13th DAA, Yuba Sutter Fair</t>
         </is>
       </c>
-      <c r="G2" s="75" t="inlineStr">
+      <c r="G2" s="79" t="inlineStr">
         <is>
           <t>14th DAA, Santa Cruz County Fair</t>
         </is>
       </c>
-      <c r="H2" s="75" t="inlineStr">
+      <c r="H2" s="79" t="inlineStr">
         <is>
           <t>17th DAA, Nevada County Fair</t>
         </is>
       </c>
-      <c r="I2" s="75" t="inlineStr">
+      <c r="I2" s="79" t="inlineStr">
         <is>
           <t>21-A DAA, Madera District Fair</t>
         </is>
       </c>
-      <c r="J2" s="75" t="inlineStr">
+      <c r="J2" s="79" t="inlineStr">
         <is>
           <t>23rd DAA, Contra Costa County Fair</t>
         </is>
       </c>
-      <c r="K2" s="75" t="inlineStr">
+      <c r="K2" s="79" t="inlineStr">
         <is>
           <t>25th DAA, Napa Town &amp; Country Fair</t>
         </is>
       </c>
-      <c r="L2" s="75" t="inlineStr">
+      <c r="L2" s="79" t="inlineStr">
         <is>
           <t>27th DAA, Shasta District Fair</t>
         </is>
       </c>
-      <c r="M2" s="75" t="inlineStr">
+      <c r="M2" s="79" t="inlineStr">
         <is>
           <t>35th DAA, Merced County Fair</t>
         </is>
       </c>
-      <c r="N2" s="75" t="inlineStr">
+      <c r="N2" s="79" t="inlineStr">
         <is>
           <t>45th DAA, CA Mid- Winter Fair</t>
         </is>
       </c>
-      <c r="O2" s="75" t="inlineStr">
+      <c r="O2" s="79" t="inlineStr">
         <is>
           <t>El Dorado County Fair</t>
         </is>
       </c>
-      <c r="P2" s="75" t="inlineStr">
+      <c r="P2" s="79" t="inlineStr">
         <is>
           <t>Humboldt County Fair</t>
         </is>
       </c>
-      <c r="Q2" s="75" t="inlineStr">
+      <c r="Q2" s="79" t="inlineStr">
         <is>
           <t>Marin County Fair</t>
         </is>
       </c>
-      <c r="R2" s="75" t="inlineStr">
+      <c r="R2" s="79" t="inlineStr">
         <is>
           <t>Salinas Valley Fair</t>
         </is>
       </c>
-      <c r="S2" s="75" t="inlineStr">
+      <c r="S2" s="79" t="inlineStr">
         <is>
           <t>Napa County Fair</t>
         </is>
       </c>
-      <c r="T2" s="75" t="inlineStr">
+      <c r="T2" s="79" t="inlineStr">
         <is>
           <t>Placer County Fair</t>
         </is>
       </c>
-      <c r="U2" s="75" t="inlineStr">
+      <c r="U2" s="79" t="inlineStr">
         <is>
           <t>Lodi Grape Festival</t>
         </is>
@@ -9900,29 +9900,29 @@
     <row r="3" ht="37.5" customHeight="1">
       <c r="A3" s="82" t="n"/>
       <c r="B3" s="83" t="n"/>
-      <c r="C3" s="76" t="n"/>
-      <c r="D3" s="76" t="n"/>
-      <c r="E3" s="76" t="n"/>
-      <c r="F3" s="76" t="n"/>
-      <c r="G3" s="76" t="n"/>
-      <c r="H3" s="76" t="n"/>
-      <c r="I3" s="76" t="n"/>
-      <c r="J3" s="76" t="n"/>
-      <c r="K3" s="76" t="n"/>
-      <c r="L3" s="76" t="n"/>
-      <c r="M3" s="76" t="n"/>
-      <c r="N3" s="76" t="n"/>
-      <c r="O3" s="76" t="n"/>
-      <c r="P3" s="76" t="n"/>
-      <c r="Q3" s="76" t="n"/>
-      <c r="R3" s="76" t="n"/>
-      <c r="S3" s="76" t="n"/>
-      <c r="T3" s="76" t="n"/>
-      <c r="U3" s="76" t="n"/>
+      <c r="C3" s="80" t="n"/>
+      <c r="D3" s="80" t="n"/>
+      <c r="E3" s="80" t="n"/>
+      <c r="F3" s="80" t="n"/>
+      <c r="G3" s="80" t="n"/>
+      <c r="H3" s="80" t="n"/>
+      <c r="I3" s="80" t="n"/>
+      <c r="J3" s="80" t="n"/>
+      <c r="K3" s="80" t="n"/>
+      <c r="L3" s="80" t="n"/>
+      <c r="M3" s="80" t="n"/>
+      <c r="N3" s="80" t="n"/>
+      <c r="O3" s="80" t="n"/>
+      <c r="P3" s="80" t="n"/>
+      <c r="Q3" s="80" t="n"/>
+      <c r="R3" s="80" t="n"/>
+      <c r="S3" s="80" t="n"/>
+      <c r="T3" s="80" t="n"/>
+      <c r="U3" s="80" t="n"/>
     </row>
     <row r="4" ht="15" customHeight="1">
-      <c r="A4" s="79" t="n"/>
-      <c r="B4" s="80" t="n"/>
+      <c r="A4" s="77" t="n"/>
+      <c r="B4" s="78" t="n"/>
       <c r="C4" s="2" t="n"/>
       <c r="D4" s="2" t="n"/>
       <c r="E4" s="2" t="n"/>
@@ -12387,8 +12387,8 @@
       <c r="U47" s="36" t="n"/>
     </row>
     <row r="48">
-      <c r="A48" s="77" t="n"/>
-      <c r="B48" s="78" t="n"/>
+      <c r="A48" s="75" t="n"/>
+      <c r="B48" s="76" t="n"/>
       <c r="C48" s="1" t="n"/>
       <c r="D48" s="1" t="n"/>
       <c r="E48" s="1" t="n"/>
@@ -12410,8 +12410,8 @@
       <c r="U48" s="1" t="n"/>
     </row>
     <row r="49" ht="66" customHeight="1">
-      <c r="A49" s="79" t="n"/>
-      <c r="B49" s="80" t="n"/>
+      <c r="A49" s="77" t="n"/>
+      <c r="B49" s="78" t="n"/>
       <c r="C49" s="16" t="inlineStr">
         <is>
           <t>3rd DAA, Silver Dollar Fair</t>
@@ -12515,25 +12515,25 @@
         </is>
       </c>
       <c r="B50" s="6" t="n"/>
-      <c r="C50" s="77" t="n"/>
-      <c r="D50" s="77" t="n"/>
-      <c r="E50" s="77" t="n"/>
-      <c r="F50" s="77" t="n"/>
-      <c r="G50" s="77" t="n"/>
-      <c r="H50" s="77" t="n"/>
-      <c r="I50" s="77" t="n"/>
-      <c r="J50" s="77" t="n"/>
-      <c r="K50" s="77" t="n"/>
-      <c r="L50" s="77" t="n"/>
-      <c r="M50" s="77" t="n"/>
-      <c r="N50" s="77" t="n"/>
-      <c r="O50" s="77" t="n"/>
-      <c r="P50" s="77" t="n"/>
-      <c r="Q50" s="77" t="n"/>
-      <c r="R50" s="77" t="n"/>
-      <c r="S50" s="77" t="n"/>
-      <c r="T50" s="77" t="n"/>
-      <c r="U50" s="77" t="n"/>
+      <c r="C50" s="75" t="n"/>
+      <c r="D50" s="75" t="n"/>
+      <c r="E50" s="75" t="n"/>
+      <c r="F50" s="75" t="n"/>
+      <c r="G50" s="75" t="n"/>
+      <c r="H50" s="75" t="n"/>
+      <c r="I50" s="75" t="n"/>
+      <c r="J50" s="75" t="n"/>
+      <c r="K50" s="75" t="n"/>
+      <c r="L50" s="75" t="n"/>
+      <c r="M50" s="75" t="n"/>
+      <c r="N50" s="75" t="n"/>
+      <c r="O50" s="75" t="n"/>
+      <c r="P50" s="75" t="n"/>
+      <c r="Q50" s="75" t="n"/>
+      <c r="R50" s="75" t="n"/>
+      <c r="S50" s="75" t="n"/>
+      <c r="T50" s="75" t="n"/>
+      <c r="U50" s="75" t="n"/>
     </row>
     <row r="51">
       <c r="A51" s="3" t="inlineStr">
@@ -12542,25 +12542,25 @@
         </is>
       </c>
       <c r="B51" s="6" t="n"/>
-      <c r="C51" s="77" t="n"/>
-      <c r="D51" s="77" t="n"/>
-      <c r="E51" s="77" t="n"/>
-      <c r="F51" s="77" t="n"/>
-      <c r="G51" s="77" t="n"/>
-      <c r="H51" s="77" t="n"/>
-      <c r="I51" s="77" t="n"/>
-      <c r="J51" s="77" t="n"/>
-      <c r="K51" s="77" t="n"/>
-      <c r="L51" s="77" t="n"/>
-      <c r="M51" s="77" t="n"/>
-      <c r="N51" s="77" t="n"/>
-      <c r="O51" s="77" t="n"/>
-      <c r="P51" s="77" t="n"/>
-      <c r="Q51" s="77" t="n"/>
-      <c r="R51" s="77" t="n"/>
-      <c r="S51" s="77" t="n"/>
-      <c r="T51" s="77" t="n"/>
-      <c r="U51" s="77" t="n"/>
+      <c r="C51" s="75" t="n"/>
+      <c r="D51" s="75" t="n"/>
+      <c r="E51" s="75" t="n"/>
+      <c r="F51" s="75" t="n"/>
+      <c r="G51" s="75" t="n"/>
+      <c r="H51" s="75" t="n"/>
+      <c r="I51" s="75" t="n"/>
+      <c r="J51" s="75" t="n"/>
+      <c r="K51" s="75" t="n"/>
+      <c r="L51" s="75" t="n"/>
+      <c r="M51" s="75" t="n"/>
+      <c r="N51" s="75" t="n"/>
+      <c r="O51" s="75" t="n"/>
+      <c r="P51" s="75" t="n"/>
+      <c r="Q51" s="75" t="n"/>
+      <c r="R51" s="75" t="n"/>
+      <c r="S51" s="75" t="n"/>
+      <c r="T51" s="75" t="n"/>
+      <c r="U51" s="75" t="n"/>
     </row>
     <row r="52">
       <c r="A52" s="5" t="n"/>
@@ -13143,25 +13143,25 @@
         </is>
       </c>
       <c r="B62" s="6" t="n"/>
-      <c r="C62" s="77" t="n"/>
-      <c r="D62" s="77" t="n"/>
-      <c r="E62" s="77" t="n"/>
-      <c r="F62" s="77" t="n"/>
-      <c r="G62" s="77" t="n"/>
-      <c r="H62" s="77" t="n"/>
-      <c r="I62" s="77" t="n"/>
-      <c r="J62" s="77" t="n"/>
-      <c r="K62" s="77" t="n"/>
-      <c r="L62" s="77" t="n"/>
-      <c r="M62" s="77" t="n"/>
-      <c r="N62" s="77" t="n"/>
-      <c r="O62" s="77" t="n"/>
-      <c r="P62" s="77" t="n"/>
-      <c r="Q62" s="77" t="n"/>
-      <c r="R62" s="77" t="n"/>
-      <c r="S62" s="77" t="n"/>
-      <c r="T62" s="77" t="n"/>
-      <c r="U62" s="77" t="n"/>
+      <c r="C62" s="75" t="n"/>
+      <c r="D62" s="75" t="n"/>
+      <c r="E62" s="75" t="n"/>
+      <c r="F62" s="75" t="n"/>
+      <c r="G62" s="75" t="n"/>
+      <c r="H62" s="75" t="n"/>
+      <c r="I62" s="75" t="n"/>
+      <c r="J62" s="75" t="n"/>
+      <c r="K62" s="75" t="n"/>
+      <c r="L62" s="75" t="n"/>
+      <c r="M62" s="75" t="n"/>
+      <c r="N62" s="75" t="n"/>
+      <c r="O62" s="75" t="n"/>
+      <c r="P62" s="75" t="n"/>
+      <c r="Q62" s="75" t="n"/>
+      <c r="R62" s="75" t="n"/>
+      <c r="S62" s="75" t="n"/>
+      <c r="T62" s="75" t="n"/>
+      <c r="U62" s="75" t="n"/>
     </row>
     <row r="63">
       <c r="A63" s="5" t="n"/>
@@ -13648,25 +13648,25 @@
         </is>
       </c>
       <c r="B71" s="6" t="n"/>
-      <c r="C71" s="77" t="n"/>
-      <c r="D71" s="77" t="n"/>
-      <c r="E71" s="77" t="n"/>
-      <c r="F71" s="77" t="n"/>
-      <c r="G71" s="77" t="n"/>
-      <c r="H71" s="77" t="n"/>
-      <c r="I71" s="77" t="n"/>
-      <c r="J71" s="77" t="n"/>
-      <c r="K71" s="77" t="n"/>
-      <c r="L71" s="77" t="n"/>
-      <c r="M71" s="77" t="n"/>
-      <c r="N71" s="77" t="n"/>
-      <c r="O71" s="77" t="n"/>
-      <c r="P71" s="77" t="n"/>
-      <c r="Q71" s="77" t="n"/>
-      <c r="R71" s="77" t="n"/>
-      <c r="S71" s="77" t="n"/>
-      <c r="T71" s="77" t="n"/>
-      <c r="U71" s="77" t="n"/>
+      <c r="C71" s="75" t="n"/>
+      <c r="D71" s="75" t="n"/>
+      <c r="E71" s="75" t="n"/>
+      <c r="F71" s="75" t="n"/>
+      <c r="G71" s="75" t="n"/>
+      <c r="H71" s="75" t="n"/>
+      <c r="I71" s="75" t="n"/>
+      <c r="J71" s="75" t="n"/>
+      <c r="K71" s="75" t="n"/>
+      <c r="L71" s="75" t="n"/>
+      <c r="M71" s="75" t="n"/>
+      <c r="N71" s="75" t="n"/>
+      <c r="O71" s="75" t="n"/>
+      <c r="P71" s="75" t="n"/>
+      <c r="Q71" s="75" t="n"/>
+      <c r="R71" s="75" t="n"/>
+      <c r="S71" s="75" t="n"/>
+      <c r="T71" s="75" t="n"/>
+      <c r="U71" s="75" t="n"/>
     </row>
     <row r="72">
       <c r="A72" s="5" t="n"/>
@@ -14033,6 +14033,19 @@
     </row>
   </sheetData>
   <mergeCells count="21">
+    <mergeCell ref="S2:S3"/>
+    <mergeCell ref="T2:T3"/>
+    <mergeCell ref="U2:U3"/>
+    <mergeCell ref="O2:O3"/>
+    <mergeCell ref="P2:P3"/>
+    <mergeCell ref="Q2:Q3"/>
+    <mergeCell ref="R2:R3"/>
+    <mergeCell ref="K2:K3"/>
+    <mergeCell ref="L2:L3"/>
+    <mergeCell ref="M2:M3"/>
+    <mergeCell ref="N2:N3"/>
+    <mergeCell ref="D2:D3"/>
+    <mergeCell ref="E2:E3"/>
     <mergeCell ref="A1:B4"/>
     <mergeCell ref="A48:B49"/>
     <mergeCell ref="C2:C3"/>
@@ -14041,19 +14054,6 @@
     <mergeCell ref="G2:G3"/>
     <mergeCell ref="H2:H3"/>
     <mergeCell ref="I2:I3"/>
-    <mergeCell ref="K2:K3"/>
-    <mergeCell ref="L2:L3"/>
-    <mergeCell ref="M2:M3"/>
-    <mergeCell ref="N2:N3"/>
-    <mergeCell ref="D2:D3"/>
-    <mergeCell ref="E2:E3"/>
-    <mergeCell ref="S2:S3"/>
-    <mergeCell ref="T2:T3"/>
-    <mergeCell ref="U2:U3"/>
-    <mergeCell ref="O2:O3"/>
-    <mergeCell ref="P2:P3"/>
-    <mergeCell ref="Q2:Q3"/>
-    <mergeCell ref="R2:R3"/>
   </mergeCells>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.5" right="0.5" top="0.5" bottom="0.5" header="0.25" footer="0.25"/>
@@ -14090,13 +14090,13 @@
     <col width="5.140625" customWidth="1" style="15" min="1" max="1"/>
     <col width="32.28515625" customWidth="1" style="15" min="2" max="2"/>
     <col width="10.28515625" customWidth="1" style="15" min="3" max="11"/>
-    <col width="9.140625" customWidth="1" style="15" min="12" max="13"/>
-    <col width="9.140625" customWidth="1" style="15" min="14" max="16384"/>
+    <col width="9.140625" customWidth="1" style="15" min="12" max="14"/>
+    <col width="9.140625" customWidth="1" style="15" min="15" max="16384"/>
   </cols>
   <sheetData>
     <row r="1">
       <c r="A1" s="81" t="n"/>
-      <c r="B1" s="78" t="n"/>
+      <c r="B1" s="76" t="n"/>
       <c r="C1" s="1" t="n"/>
       <c r="D1" s="1" t="n"/>
       <c r="E1" s="1" t="n"/>
@@ -14110,48 +14110,48 @@
     <row r="2">
       <c r="A2" s="82" t="n"/>
       <c r="B2" s="83" t="n"/>
-      <c r="C2" s="75" t="inlineStr">
+      <c r="C2" s="79" t="inlineStr">
         <is>
           <t>7th DAA, Monterey County Fair</t>
         </is>
       </c>
-      <c r="D2" s="75" t="inlineStr">
+      <c r="D2" s="79" t="inlineStr">
         <is>
           <t>19th DAA, Santa Barbara Fair</t>
         </is>
       </c>
-      <c r="E2" s="75" t="inlineStr">
+      <c r="E2" s="79" t="inlineStr">
         <is>
           <t>24th DAA, Tulare County Fair</t>
         </is>
       </c>
-      <c r="F2" s="75" t="inlineStr">
+      <c r="F2" s="79" t="inlineStr">
         <is>
           <t>28th DAA, San Bernardino County Fair</t>
         </is>
       </c>
-      <c r="G2" s="75" t="inlineStr">
+      <c r="G2" s="79" t="inlineStr">
         <is>
           <t>37th DAA, Santa Maria Fair Park</t>
         </is>
       </c>
-      <c r="H2" s="75" t="inlineStr">
+      <c r="H2" s="79" t="inlineStr">
         <is>
           <t>38th DAA, Stanislaus County Fair</t>
         </is>
       </c>
-      <c r="I2" s="75" t="inlineStr">
+      <c r="I2" s="79" t="inlineStr">
         <is>
           <t>46th DAA, Farmers Fair &amp; Festival</t>
         </is>
       </c>
-      <c r="J2" s="75" t="inlineStr">
+      <c r="J2" s="79" t="inlineStr">
         <is>
           <t>National Date Festival 
 (FY 00/01)</t>
         </is>
       </c>
-      <c r="K2" s="75" t="inlineStr">
+      <c r="K2" s="79" t="inlineStr">
         <is>
           <t>San Mateo County Fair</t>
         </is>
@@ -14160,19 +14160,19 @@
     <row r="3" ht="37.5" customHeight="1">
       <c r="A3" s="82" t="n"/>
       <c r="B3" s="83" t="n"/>
-      <c r="C3" s="76" t="n"/>
-      <c r="D3" s="76" t="n"/>
-      <c r="E3" s="76" t="n"/>
-      <c r="F3" s="76" t="n"/>
-      <c r="G3" s="76" t="n"/>
-      <c r="H3" s="76" t="n"/>
-      <c r="I3" s="76" t="n"/>
-      <c r="J3" s="76" t="n"/>
-      <c r="K3" s="76" t="n"/>
+      <c r="C3" s="80" t="n"/>
+      <c r="D3" s="80" t="n"/>
+      <c r="E3" s="80" t="n"/>
+      <c r="F3" s="80" t="n"/>
+      <c r="G3" s="80" t="n"/>
+      <c r="H3" s="80" t="n"/>
+      <c r="I3" s="80" t="n"/>
+      <c r="J3" s="80" t="n"/>
+      <c r="K3" s="80" t="n"/>
     </row>
     <row r="4" ht="14.25" customHeight="1">
-      <c r="A4" s="79" t="n"/>
-      <c r="B4" s="80" t="n"/>
+      <c r="A4" s="77" t="n"/>
+      <c r="B4" s="78" t="n"/>
       <c r="C4" s="2" t="n"/>
       <c r="D4" s="2" t="n"/>
       <c r="E4" s="2" t="n"/>
@@ -15556,8 +15556,8 @@
       <c r="K48" s="36" t="n"/>
     </row>
     <row r="49">
-      <c r="A49" s="77" t="n"/>
-      <c r="B49" s="78" t="n"/>
+      <c r="A49" s="75" t="n"/>
+      <c r="B49" s="76" t="n"/>
       <c r="C49" s="1" t="n"/>
       <c r="D49" s="1" t="n"/>
       <c r="E49" s="1" t="n"/>
@@ -15569,8 +15569,8 @@
       <c r="K49" s="1" t="n"/>
     </row>
     <row r="50" ht="66" customHeight="1">
-      <c r="A50" s="79" t="n"/>
-      <c r="B50" s="80" t="n"/>
+      <c r="A50" s="77" t="n"/>
+      <c r="B50" s="78" t="n"/>
       <c r="C50" s="16" t="inlineStr">
         <is>
           <t>7th DAA, Monterey County Fair</t>
@@ -15625,15 +15625,15 @@
         </is>
       </c>
       <c r="B51" s="6" t="n"/>
-      <c r="C51" s="77" t="n"/>
-      <c r="D51" s="77" t="n"/>
-      <c r="E51" s="77" t="n"/>
-      <c r="F51" s="77" t="n"/>
-      <c r="G51" s="77" t="n"/>
-      <c r="H51" s="77" t="n"/>
-      <c r="I51" s="77" t="n"/>
-      <c r="J51" s="77" t="n"/>
-      <c r="K51" s="77" t="n"/>
+      <c r="C51" s="75" t="n"/>
+      <c r="D51" s="75" t="n"/>
+      <c r="E51" s="75" t="n"/>
+      <c r="F51" s="75" t="n"/>
+      <c r="G51" s="75" t="n"/>
+      <c r="H51" s="75" t="n"/>
+      <c r="I51" s="75" t="n"/>
+      <c r="J51" s="75" t="n"/>
+      <c r="K51" s="75" t="n"/>
     </row>
     <row r="52">
       <c r="A52" s="3" t="inlineStr">
@@ -15642,15 +15642,15 @@
         </is>
       </c>
       <c r="B52" s="6" t="n"/>
-      <c r="C52" s="77" t="n"/>
-      <c r="D52" s="77" t="n"/>
-      <c r="E52" s="77" t="n"/>
-      <c r="F52" s="77" t="n"/>
-      <c r="G52" s="77" t="n"/>
-      <c r="H52" s="77" t="n"/>
-      <c r="I52" s="77" t="n"/>
-      <c r="J52" s="77" t="n"/>
-      <c r="K52" s="77" t="n"/>
+      <c r="C52" s="75" t="n"/>
+      <c r="D52" s="75" t="n"/>
+      <c r="E52" s="75" t="n"/>
+      <c r="F52" s="75" t="n"/>
+      <c r="G52" s="75" t="n"/>
+      <c r="H52" s="75" t="n"/>
+      <c r="I52" s="75" t="n"/>
+      <c r="J52" s="75" t="n"/>
+      <c r="K52" s="75" t="n"/>
     </row>
     <row r="53">
       <c r="A53" s="5" t="n"/>
@@ -15973,15 +15973,15 @@
         </is>
       </c>
       <c r="B63" s="6" t="n"/>
-      <c r="C63" s="77" t="n"/>
-      <c r="D63" s="77" t="n"/>
-      <c r="E63" s="77" t="n"/>
-      <c r="F63" s="77" t="n"/>
-      <c r="G63" s="77" t="n"/>
-      <c r="H63" s="77" t="n"/>
-      <c r="I63" s="77" t="n"/>
-      <c r="J63" s="77" t="n"/>
-      <c r="K63" s="77" t="n"/>
+      <c r="C63" s="75" t="n"/>
+      <c r="D63" s="75" t="n"/>
+      <c r="E63" s="75" t="n"/>
+      <c r="F63" s="75" t="n"/>
+      <c r="G63" s="75" t="n"/>
+      <c r="H63" s="75" t="n"/>
+      <c r="I63" s="75" t="n"/>
+      <c r="J63" s="75" t="n"/>
+      <c r="K63" s="75" t="n"/>
     </row>
     <row r="64">
       <c r="A64" s="5" t="n"/>
@@ -16285,15 +16285,15 @@
         </is>
       </c>
       <c r="B73" s="6" t="n"/>
-      <c r="C73" s="77" t="n"/>
-      <c r="D73" s="77" t="n"/>
-      <c r="E73" s="77" t="n"/>
-      <c r="F73" s="77" t="n"/>
-      <c r="G73" s="77" t="n"/>
-      <c r="H73" s="77" t="n"/>
-      <c r="I73" s="77" t="n"/>
-      <c r="J73" s="77" t="n"/>
-      <c r="K73" s="77" t="n"/>
+      <c r="C73" s="75" t="n"/>
+      <c r="D73" s="75" t="n"/>
+      <c r="E73" s="75" t="n"/>
+      <c r="F73" s="75" t="n"/>
+      <c r="G73" s="75" t="n"/>
+      <c r="H73" s="75" t="n"/>
+      <c r="I73" s="75" t="n"/>
+      <c r="J73" s="75" t="n"/>
+      <c r="K73" s="75" t="n"/>
     </row>
     <row r="74">
       <c r="A74" s="5" t="n"/>
@@ -16492,17 +16492,17 @@
     </row>
   </sheetData>
   <mergeCells count="11">
-    <mergeCell ref="A49:B50"/>
-    <mergeCell ref="C2:C3"/>
-    <mergeCell ref="D2:D3"/>
-    <mergeCell ref="E2:E3"/>
-    <mergeCell ref="A1:B4"/>
     <mergeCell ref="K2:K3"/>
     <mergeCell ref="J2:J3"/>
     <mergeCell ref="F2:F3"/>
     <mergeCell ref="G2:G3"/>
     <mergeCell ref="H2:H3"/>
     <mergeCell ref="I2:I3"/>
+    <mergeCell ref="A49:B50"/>
+    <mergeCell ref="C2:C3"/>
+    <mergeCell ref="D2:D3"/>
+    <mergeCell ref="E2:E3"/>
+    <mergeCell ref="A1:B4"/>
   </mergeCells>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.5" right="0.5" top="0.4" bottom="0.4" header="0.25" footer="0.25"/>
@@ -16540,13 +16540,13 @@
     <col width="11" customWidth="1" style="15" min="6" max="6"/>
     <col width="11.42578125" customWidth="1" style="15" min="7" max="7"/>
     <col width="11" customWidth="1" style="15" min="8" max="8"/>
-    <col width="9.140625" customWidth="1" style="15" min="9" max="10"/>
-    <col width="9.140625" customWidth="1" style="15" min="11" max="16384"/>
+    <col width="9.140625" customWidth="1" style="15" min="9" max="11"/>
+    <col width="9.140625" customWidth="1" style="15" min="12" max="16384"/>
   </cols>
   <sheetData>
     <row r="1">
       <c r="A1" s="81" t="n"/>
-      <c r="B1" s="78" t="n"/>
+      <c r="B1" s="76" t="n"/>
       <c r="C1" s="1" t="n"/>
       <c r="D1" s="1" t="n"/>
       <c r="E1" s="1" t="n"/>
@@ -16557,32 +16557,32 @@
     <row r="2">
       <c r="A2" s="82" t="n"/>
       <c r="B2" s="83" t="n"/>
-      <c r="C2" s="75" t="inlineStr">
+      <c r="C2" s="79" t="inlineStr">
         <is>
           <t>2nd DAA, San Joaquin County Fair</t>
         </is>
       </c>
-      <c r="D2" s="75" t="inlineStr">
+      <c r="D2" s="79" t="inlineStr">
         <is>
           <t>15th DAA, Kern County Fair</t>
         </is>
       </c>
-      <c r="E2" s="75" t="inlineStr">
+      <c r="E2" s="79" t="inlineStr">
         <is>
           <t>16th DAA, CA Mid- State Fair</t>
         </is>
       </c>
-      <c r="F2" s="75" t="inlineStr">
+      <c r="F2" s="79" t="inlineStr">
         <is>
           <t>31st DAA, Ventura County Fair</t>
         </is>
       </c>
-      <c r="G2" s="75" t="inlineStr">
+      <c r="G2" s="79" t="inlineStr">
         <is>
           <t>50th DAA, Antelope Valley Fair</t>
         </is>
       </c>
-      <c r="H2" s="75" t="inlineStr">
+      <c r="H2" s="79" t="inlineStr">
         <is>
           <t>Solano County Fair</t>
         </is>
@@ -16591,16 +16591,16 @@
     <row r="3" ht="37.5" customHeight="1">
       <c r="A3" s="82" t="n"/>
       <c r="B3" s="83" t="n"/>
-      <c r="C3" s="76" t="n"/>
-      <c r="D3" s="76" t="n"/>
-      <c r="E3" s="76" t="n"/>
-      <c r="F3" s="76" t="n"/>
-      <c r="G3" s="76" t="n"/>
-      <c r="H3" s="76" t="n"/>
+      <c r="C3" s="80" t="n"/>
+      <c r="D3" s="80" t="n"/>
+      <c r="E3" s="80" t="n"/>
+      <c r="F3" s="80" t="n"/>
+      <c r="G3" s="80" t="n"/>
+      <c r="H3" s="80" t="n"/>
     </row>
     <row r="4" ht="14.25" customHeight="1">
-      <c r="A4" s="79" t="n"/>
-      <c r="B4" s="80" t="n"/>
+      <c r="A4" s="77" t="n"/>
+      <c r="B4" s="78" t="n"/>
       <c r="C4" s="2" t="n"/>
       <c r="D4" s="2" t="n"/>
       <c r="E4" s="2" t="n"/>
@@ -17639,8 +17639,8 @@
       <c r="H48" s="36" t="n"/>
     </row>
     <row r="49">
-      <c r="A49" s="77" t="n"/>
-      <c r="B49" s="78" t="n"/>
+      <c r="A49" s="75" t="n"/>
+      <c r="B49" s="76" t="n"/>
       <c r="C49" s="1" t="n"/>
       <c r="D49" s="1" t="n"/>
       <c r="E49" s="1" t="n"/>
@@ -17649,8 +17649,8 @@
       <c r="H49" s="1" t="n"/>
     </row>
     <row r="50" ht="66" customHeight="1">
-      <c r="A50" s="79" t="n"/>
-      <c r="B50" s="80" t="n"/>
+      <c r="A50" s="77" t="n"/>
+      <c r="B50" s="78" t="n"/>
       <c r="C50" s="16" t="inlineStr">
         <is>
           <t>2nd DAA, San Joaquin County Fair</t>
@@ -17689,12 +17689,12 @@
         </is>
       </c>
       <c r="B51" s="6" t="n"/>
-      <c r="C51" s="77" t="n"/>
-      <c r="D51" s="77" t="n"/>
-      <c r="E51" s="77" t="n"/>
-      <c r="F51" s="77" t="n"/>
-      <c r="G51" s="77" t="n"/>
-      <c r="H51" s="77" t="n"/>
+      <c r="C51" s="75" t="n"/>
+      <c r="D51" s="75" t="n"/>
+      <c r="E51" s="75" t="n"/>
+      <c r="F51" s="75" t="n"/>
+      <c r="G51" s="75" t="n"/>
+      <c r="H51" s="75" t="n"/>
     </row>
     <row r="52">
       <c r="A52" s="3" t="inlineStr">
@@ -17703,12 +17703,12 @@
         </is>
       </c>
       <c r="B52" s="6" t="n"/>
-      <c r="C52" s="77" t="n"/>
-      <c r="D52" s="77" t="n"/>
-      <c r="E52" s="77" t="n"/>
-      <c r="F52" s="77" t="n"/>
-      <c r="G52" s="77" t="n"/>
-      <c r="H52" s="77" t="n"/>
+      <c r="C52" s="75" t="n"/>
+      <c r="D52" s="75" t="n"/>
+      <c r="E52" s="75" t="n"/>
+      <c r="F52" s="75" t="n"/>
+      <c r="G52" s="75" t="n"/>
+      <c r="H52" s="75" t="n"/>
     </row>
     <row r="53">
       <c r="A53" s="5" t="n"/>
@@ -17953,12 +17953,12 @@
         </is>
       </c>
       <c r="B63" s="6" t="n"/>
-      <c r="C63" s="77" t="n"/>
-      <c r="D63" s="77" t="n"/>
-      <c r="E63" s="77" t="n"/>
-      <c r="F63" s="77" t="n"/>
-      <c r="G63" s="77" t="n"/>
-      <c r="H63" s="77" t="n"/>
+      <c r="C63" s="75" t="n"/>
+      <c r="D63" s="75" t="n"/>
+      <c r="E63" s="75" t="n"/>
+      <c r="F63" s="75" t="n"/>
+      <c r="G63" s="75" t="n"/>
+      <c r="H63" s="75" t="n"/>
     </row>
     <row r="64">
       <c r="A64" s="5" t="n"/>
@@ -18163,12 +18163,12 @@
         </is>
       </c>
       <c r="B72" s="6" t="n"/>
-      <c r="C72" s="77" t="n"/>
-      <c r="D72" s="77" t="n"/>
-      <c r="E72" s="77" t="n"/>
-      <c r="F72" s="77" t="n"/>
-      <c r="G72" s="77" t="n"/>
-      <c r="H72" s="77" t="n"/>
+      <c r="C72" s="75" t="n"/>
+      <c r="D72" s="75" t="n"/>
+      <c r="E72" s="75" t="n"/>
+      <c r="F72" s="75" t="n"/>
+      <c r="G72" s="75" t="n"/>
+      <c r="H72" s="75" t="n"/>
     </row>
     <row r="73">
       <c r="A73" s="5" t="n"/>
@@ -18373,13 +18373,13 @@
     <col width="11.140625" customWidth="1" style="15" min="6" max="6"/>
     <col width="11.28515625" customWidth="1" style="15" min="7" max="8"/>
     <col width="10.28515625" customWidth="1" style="15" min="9" max="10"/>
-    <col width="9.140625" customWidth="1" style="15" min="11" max="12"/>
-    <col width="9.140625" customWidth="1" style="15" min="13" max="16384"/>
+    <col width="9.140625" customWidth="1" style="15" min="11" max="13"/>
+    <col width="9.140625" customWidth="1" style="15" min="14" max="16384"/>
   </cols>
   <sheetData>
     <row r="1">
       <c r="A1" s="81" t="n"/>
-      <c r="B1" s="78" t="n"/>
+      <c r="B1" s="76" t="n"/>
       <c r="C1" s="1" t="n"/>
       <c r="D1" s="1" t="n"/>
       <c r="E1" s="1" t="n"/>
@@ -18390,32 +18390,32 @@
     <row r="2">
       <c r="A2" s="82" t="n"/>
       <c r="B2" s="83" t="n"/>
-      <c r="C2" s="75" t="inlineStr">
+      <c r="C2" s="79" t="inlineStr">
         <is>
           <t>1-A DAA, Grand Nat'l Rodeo &amp; Show (FY 00/01)</t>
         </is>
       </c>
-      <c r="D2" s="75" t="inlineStr">
+      <c r="D2" s="79" t="inlineStr">
         <is>
           <t>21st DAA, The Big Fresno Fair</t>
         </is>
       </c>
-      <c r="E2" s="75" t="inlineStr">
+      <c r="E2" s="79" t="inlineStr">
         <is>
           <t>Alameda County Fair</t>
         </is>
       </c>
-      <c r="F2" s="75" t="inlineStr">
+      <c r="F2" s="79" t="inlineStr">
         <is>
           <t>National Orange Show</t>
         </is>
       </c>
-      <c r="G2" s="75" t="inlineStr">
+      <c r="G2" s="79" t="inlineStr">
         <is>
           <t>Santa Clara County Fair</t>
         </is>
       </c>
-      <c r="H2" s="75" t="inlineStr">
+      <c r="H2" s="79" t="inlineStr">
         <is>
           <t>Sonoma County Fair</t>
         </is>
@@ -18424,16 +18424,16 @@
     <row r="3" ht="36.75" customHeight="1">
       <c r="A3" s="82" t="n"/>
       <c r="B3" s="83" t="n"/>
-      <c r="C3" s="76" t="n"/>
-      <c r="D3" s="76" t="n"/>
-      <c r="E3" s="76" t="n"/>
-      <c r="F3" s="76" t="n"/>
-      <c r="G3" s="76" t="n"/>
-      <c r="H3" s="76" t="n"/>
+      <c r="C3" s="80" t="n"/>
+      <c r="D3" s="80" t="n"/>
+      <c r="E3" s="80" t="n"/>
+      <c r="F3" s="80" t="n"/>
+      <c r="G3" s="80" t="n"/>
+      <c r="H3" s="80" t="n"/>
     </row>
     <row r="4" ht="8.25" customHeight="1">
-      <c r="A4" s="79" t="n"/>
-      <c r="B4" s="80" t="n"/>
+      <c r="A4" s="77" t="n"/>
+      <c r="B4" s="78" t="n"/>
       <c r="C4" s="2" t="n"/>
       <c r="D4" s="2" t="n"/>
       <c r="E4" s="2" t="n"/>
@@ -19550,8 +19550,8 @@
       <c r="H51" s="36" t="n"/>
     </row>
     <row r="52">
-      <c r="A52" s="77" t="n"/>
-      <c r="B52" s="78" t="n"/>
+      <c r="A52" s="75" t="n"/>
+      <c r="B52" s="76" t="n"/>
       <c r="C52" s="1" t="n"/>
       <c r="D52" s="1" t="n"/>
       <c r="E52" s="1" t="n"/>
@@ -19560,8 +19560,8 @@
       <c r="H52" s="1" t="n"/>
     </row>
     <row r="53" ht="66" customHeight="1">
-      <c r="A53" s="79" t="n"/>
-      <c r="B53" s="80" t="n"/>
+      <c r="A53" s="77" t="n"/>
+      <c r="B53" s="78" t="n"/>
       <c r="C53" s="16" t="inlineStr">
         <is>
           <t>1-A DAA, Grand Nat'l Rodeo &amp; Show (FY 00/01)</t>
@@ -19600,12 +19600,12 @@
         </is>
       </c>
       <c r="B54" s="6" t="n"/>
-      <c r="C54" s="77" t="n"/>
-      <c r="D54" s="77" t="n"/>
-      <c r="E54" s="77" t="n"/>
-      <c r="F54" s="77" t="n"/>
-      <c r="G54" s="77" t="n"/>
-      <c r="H54" s="77" t="n"/>
+      <c r="C54" s="75" t="n"/>
+      <c r="D54" s="75" t="n"/>
+      <c r="E54" s="75" t="n"/>
+      <c r="F54" s="75" t="n"/>
+      <c r="G54" s="75" t="n"/>
+      <c r="H54" s="75" t="n"/>
     </row>
     <row r="55">
       <c r="A55" s="3" t="inlineStr">
@@ -19614,12 +19614,12 @@
         </is>
       </c>
       <c r="B55" s="6" t="n"/>
-      <c r="C55" s="77" t="n"/>
-      <c r="D55" s="77" t="n"/>
-      <c r="E55" s="77" t="n"/>
-      <c r="F55" s="77" t="n"/>
-      <c r="G55" s="77" t="n"/>
-      <c r="H55" s="77" t="n"/>
+      <c r="C55" s="75" t="n"/>
+      <c r="D55" s="75" t="n"/>
+      <c r="E55" s="75" t="n"/>
+      <c r="F55" s="75" t="n"/>
+      <c r="G55" s="75" t="n"/>
+      <c r="H55" s="75" t="n"/>
     </row>
     <row r="56">
       <c r="A56" s="5" t="n"/>
@@ -19864,12 +19864,12 @@
         </is>
       </c>
       <c r="B66" s="6" t="n"/>
-      <c r="C66" s="77" t="n"/>
-      <c r="D66" s="77" t="n"/>
-      <c r="E66" s="77" t="n"/>
-      <c r="F66" s="77" t="n"/>
-      <c r="G66" s="77" t="n"/>
-      <c r="H66" s="77" t="n"/>
+      <c r="C66" s="75" t="n"/>
+      <c r="D66" s="75" t="n"/>
+      <c r="E66" s="75" t="n"/>
+      <c r="F66" s="75" t="n"/>
+      <c r="G66" s="75" t="n"/>
+      <c r="H66" s="75" t="n"/>
     </row>
     <row r="67">
       <c r="A67" s="5" t="n"/>
@@ -20070,12 +20070,12 @@
         </is>
       </c>
       <c r="B75" s="6" t="n"/>
-      <c r="C75" s="77" t="n"/>
-      <c r="D75" s="77" t="n"/>
-      <c r="E75" s="77" t="n"/>
-      <c r="F75" s="77" t="n"/>
-      <c r="G75" s="77" t="n"/>
-      <c r="H75" s="77" t="n"/>
+      <c r="C75" s="75" t="n"/>
+      <c r="D75" s="75" t="n"/>
+      <c r="E75" s="75" t="n"/>
+      <c r="F75" s="75" t="n"/>
+      <c r="G75" s="75" t="n"/>
+      <c r="H75" s="75" t="n"/>
     </row>
     <row r="76">
       <c r="A76" s="5" t="n"/>
@@ -20280,13 +20280,13 @@
     <col width="11.28515625" customWidth="1" style="15" min="3" max="6"/>
     <col width="2.5703125" customWidth="1" style="15" min="7" max="7"/>
     <col width="14.5703125" customWidth="1" style="15" min="8" max="8"/>
-    <col width="9.140625" customWidth="1" style="15" min="9" max="10"/>
-    <col width="9.140625" customWidth="1" style="15" min="11" max="16384"/>
+    <col width="9.140625" customWidth="1" style="15" min="9" max="11"/>
+    <col width="9.140625" customWidth="1" style="15" min="12" max="16384"/>
   </cols>
   <sheetData>
     <row r="1">
       <c r="A1" s="81" t="n"/>
-      <c r="B1" s="78" t="n"/>
+      <c r="B1" s="76" t="n"/>
       <c r="C1" s="1" t="n"/>
       <c r="D1" s="1" t="n"/>
       <c r="E1" s="32" t="n"/>
@@ -20295,22 +20295,22 @@
     <row r="2">
       <c r="A2" s="82" t="n"/>
       <c r="B2" s="83" t="n"/>
-      <c r="C2" s="75" t="inlineStr">
+      <c r="C2" s="79" t="inlineStr">
         <is>
           <t>22nd DAA, San Diego County Fair</t>
         </is>
       </c>
-      <c r="D2" s="75" t="inlineStr">
+      <c r="D2" s="79" t="inlineStr">
         <is>
           <t>32nd DAA, Orange County Fair</t>
         </is>
       </c>
-      <c r="E2" s="75" t="inlineStr">
+      <c r="E2" s="79" t="inlineStr">
         <is>
           <t>CA Exposition and State Fair (Cal Expo)</t>
         </is>
       </c>
-      <c r="F2" s="75" t="inlineStr">
+      <c r="F2" s="79" t="inlineStr">
         <is>
           <t>Los Angeles County Fair</t>
         </is>
@@ -20319,14 +20319,14 @@
     <row r="3" ht="37.5" customHeight="1">
       <c r="A3" s="82" t="n"/>
       <c r="B3" s="83" t="n"/>
-      <c r="C3" s="76" t="n"/>
-      <c r="D3" s="76" t="n"/>
-      <c r="E3" s="76" t="n"/>
-      <c r="F3" s="76" t="n"/>
+      <c r="C3" s="80" t="n"/>
+      <c r="D3" s="80" t="n"/>
+      <c r="E3" s="80" t="n"/>
+      <c r="F3" s="80" t="n"/>
     </row>
     <row r="4" ht="15" customHeight="1">
-      <c r="A4" s="79" t="n"/>
-      <c r="B4" s="80" t="n"/>
+      <c r="A4" s="77" t="n"/>
+      <c r="B4" s="78" t="n"/>
       <c r="C4" s="2" t="n"/>
       <c r="D4" s="2" t="n"/>
       <c r="E4" s="10" t="n"/>
@@ -20405,8 +20405,8 @@
       <c r="B9" s="6" t="n"/>
       <c r="C9" s="7" t="n"/>
       <c r="D9" s="7" t="n"/>
-      <c r="E9" s="77" t="n"/>
-      <c r="F9" s="77" t="n"/>
+      <c r="E9" s="75" t="n"/>
+      <c r="F9" s="75" t="n"/>
     </row>
     <row r="10">
       <c r="A10" s="5" t="n"/>
@@ -21241,16 +21241,16 @@
       <c r="D55" s="36" t="n"/>
     </row>
     <row r="56">
-      <c r="A56" s="77" t="n"/>
-      <c r="B56" s="78" t="n"/>
+      <c r="A56" s="75" t="n"/>
+      <c r="B56" s="76" t="n"/>
       <c r="C56" s="1" t="n"/>
       <c r="D56" s="1" t="n"/>
       <c r="E56" s="1" t="n"/>
       <c r="F56" s="1" t="n"/>
     </row>
     <row r="57" ht="66" customHeight="1">
-      <c r="A57" s="79" t="n"/>
-      <c r="B57" s="80" t="n"/>
+      <c r="A57" s="77" t="n"/>
+      <c r="B57" s="78" t="n"/>
       <c r="C57" s="16" t="inlineStr">
         <is>
           <t>22nd DAA, Del Mar Fair</t>
@@ -21279,10 +21279,10 @@
         </is>
       </c>
       <c r="B58" s="6" t="n"/>
-      <c r="C58" s="77" t="n"/>
-      <c r="D58" s="77" t="n"/>
-      <c r="E58" s="77" t="n"/>
-      <c r="F58" s="77" t="n"/>
+      <c r="C58" s="75" t="n"/>
+      <c r="D58" s="75" t="n"/>
+      <c r="E58" s="75" t="n"/>
+      <c r="F58" s="75" t="n"/>
     </row>
     <row r="59">
       <c r="A59" s="3" t="inlineStr">
@@ -21291,10 +21291,10 @@
         </is>
       </c>
       <c r="B59" s="6" t="n"/>
-      <c r="C59" s="77" t="n"/>
-      <c r="D59" s="77" t="n"/>
-      <c r="E59" s="77" t="n"/>
-      <c r="F59" s="77" t="n"/>
+      <c r="C59" s="75" t="n"/>
+      <c r="D59" s="75" t="n"/>
+      <c r="E59" s="75" t="n"/>
+      <c r="F59" s="75" t="n"/>
     </row>
     <row r="60">
       <c r="A60" s="5" t="n"/>
@@ -21485,10 +21485,10 @@
         </is>
       </c>
       <c r="B70" s="6" t="n"/>
-      <c r="C70" s="77" t="n"/>
-      <c r="D70" s="77" t="n"/>
-      <c r="E70" s="77" t="n"/>
-      <c r="F70" s="77" t="n"/>
+      <c r="C70" s="75" t="n"/>
+      <c r="D70" s="75" t="n"/>
+      <c r="E70" s="75" t="n"/>
+      <c r="F70" s="75" t="n"/>
     </row>
     <row r="71">
       <c r="A71" s="5" t="n"/>
@@ -21669,10 +21669,10 @@
         </is>
       </c>
       <c r="B80" s="6" t="n"/>
-      <c r="C80" s="77" t="n"/>
-      <c r="D80" s="77" t="n"/>
-      <c r="E80" s="77" t="n"/>
-      <c r="F80" s="77" t="n"/>
+      <c r="C80" s="75" t="n"/>
+      <c r="D80" s="75" t="n"/>
+      <c r="E80" s="75" t="n"/>
+      <c r="F80" s="75" t="n"/>
     </row>
     <row r="81">
       <c r="A81" s="5" t="n"/>
@@ -21839,7 +21839,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A2:BC2"/>
+  <dimension ref="A1:BC14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -21847,6 +21847,283 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>Fair Name</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>Beginning Resources 1/1/2001</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>State Allocation</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>Other</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>Admissions to Grounds</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>Industrial and Commercial Space</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>Concessions</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>Exhibits</t>
+        </is>
+      </c>
+      <c r="I1" t="inlineStr">
+        <is>
+          <t>Horse Show</t>
+        </is>
+      </c>
+      <c r="J1" t="inlineStr">
+        <is>
+          <t>Horse Racing (Fairtime Pari-Mutuel)</t>
+        </is>
+      </c>
+      <c r="K1" t="inlineStr">
+        <is>
+          <t>Horse Racing (Satellite Wagering)</t>
+        </is>
+      </c>
+      <c r="L1" t="inlineStr">
+        <is>
+          <t>Fair Attractions</t>
+        </is>
+      </c>
+      <c r="M1" t="inlineStr">
+        <is>
+          <t>Miscellaneous Fair</t>
+        </is>
+      </c>
+      <c r="N1" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Miscellaneous Non-Fair </t>
+        </is>
+      </c>
+      <c r="O1" t="inlineStr">
+        <is>
+          <t>Interim Revenue</t>
+        </is>
+      </c>
+      <c r="P1" t="inlineStr">
+        <is>
+          <t>Prior Year Revenue Adjustment</t>
+        </is>
+      </c>
+      <c r="Q1" t="inlineStr">
+        <is>
+          <t>Other Operating Revenue</t>
+        </is>
+      </c>
+      <c r="R1" t="inlineStr">
+        <is>
+          <t>Administration</t>
+        </is>
+      </c>
+      <c r="S1" t="inlineStr">
+        <is>
+          <t>Maintenance &amp; General Operations</t>
+        </is>
+      </c>
+      <c r="T1" t="inlineStr">
+        <is>
+          <t>Publicity</t>
+        </is>
+      </c>
+      <c r="U1" t="inlineStr">
+        <is>
+          <t>Attendance Operations</t>
+        </is>
+      </c>
+      <c r="V1" t="inlineStr">
+        <is>
+          <t>Miscellaneous Fair</t>
+        </is>
+      </c>
+      <c r="W1" t="inlineStr">
+        <is>
+          <t>Miscellaneous Non-Fair Programs</t>
+        </is>
+      </c>
+      <c r="X1" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Premiums </t>
+        </is>
+      </c>
+      <c r="Y1" t="inlineStr">
+        <is>
+          <t>Exhibits</t>
+        </is>
+      </c>
+      <c r="Z1" t="inlineStr">
+        <is>
+          <t>Horse Show</t>
+        </is>
+      </c>
+      <c r="AA1" t="inlineStr">
+        <is>
+          <t>Horse Racing (Fairtime Pari-Mutuel)</t>
+        </is>
+      </c>
+      <c r="AB1" t="inlineStr">
+        <is>
+          <t>Horse Racing (Satellite Wagering)</t>
+        </is>
+      </c>
+      <c r="AC1" t="inlineStr">
+        <is>
+          <t>Fair Entertainment Expense</t>
+        </is>
+      </c>
+      <c r="AD1" t="inlineStr">
+        <is>
+          <t>Interim Entertainment Expense</t>
+        </is>
+      </c>
+      <c r="AE1" t="inlineStr">
+        <is>
+          <t>Equipment Funded by Fair</t>
+        </is>
+      </c>
+      <c r="AF1" t="inlineStr">
+        <is>
+          <t>Prior Year Expense Adjustment</t>
+        </is>
+      </c>
+      <c r="AG1" t="inlineStr">
+        <is>
+          <t>Cash (Over/Under)</t>
+        </is>
+      </c>
+      <c r="AH1" t="inlineStr">
+        <is>
+          <t>Capital Expenditures Funded by Fair</t>
+        </is>
+      </c>
+      <c r="AI1" t="inlineStr">
+        <is>
+          <t>Other Addition/(Reduction) in Resources</t>
+        </is>
+      </c>
+      <c r="AJ1" t="inlineStr">
+        <is>
+          <t xml:space="preserve">    Restricted Cash</t>
+        </is>
+      </c>
+      <c r="AK1" t="inlineStr">
+        <is>
+          <t xml:space="preserve">    Available Cash</t>
+        </is>
+      </c>
+      <c r="AL1" t="inlineStr">
+        <is>
+          <t>Accounts Receivable</t>
+        </is>
+      </c>
+      <c r="AM1" t="inlineStr">
+        <is>
+          <t>Other Assets</t>
+        </is>
+      </c>
+      <c r="AN1" t="inlineStr">
+        <is>
+          <t>Land</t>
+        </is>
+      </c>
+      <c r="AO1" t="inlineStr">
+        <is>
+          <t>Buildings and Improvements</t>
+        </is>
+      </c>
+      <c r="AP1" t="inlineStr">
+        <is>
+          <t>Equipment</t>
+        </is>
+      </c>
+      <c r="AQ1" t="inlineStr">
+        <is>
+          <t>Less Accumulated Depreciation</t>
+        </is>
+      </c>
+      <c r="AR1" t="inlineStr">
+        <is>
+          <t>Insurance Fees Payable</t>
+        </is>
+      </c>
+      <c r="AS1" t="inlineStr">
+        <is>
+          <t>Accounts Payable</t>
+        </is>
+      </c>
+      <c r="AT1" t="inlineStr">
+        <is>
+          <t>Taxes &amp; Retirement Payable</t>
+        </is>
+      </c>
+      <c r="AU1" t="inlineStr">
+        <is>
+          <t>Sales Tax Payable</t>
+        </is>
+      </c>
+      <c r="AV1" t="inlineStr">
+        <is>
+          <t>Other Liabilities</t>
+        </is>
+      </c>
+      <c r="AW1" t="inlineStr">
+        <is>
+          <t>Guarantee Deposits</t>
+        </is>
+      </c>
+      <c r="AX1" t="inlineStr">
+        <is>
+          <t>Compensated Absences Liability</t>
+        </is>
+      </c>
+      <c r="AY1" t="inlineStr">
+        <is>
+          <t>Resources for Junior Livestock Auction</t>
+        </is>
+      </c>
+      <c r="AZ1" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Investment in Capital Assets </t>
+        </is>
+      </c>
+      <c r="BA1" t="inlineStr">
+        <is>
+          <t>Resources Available for Operations</t>
+        </is>
+      </c>
+      <c r="BB1" t="inlineStr">
+        <is>
+          <t>Resources Available for Projects</t>
+        </is>
+      </c>
+      <c r="BC1" t="inlineStr">
+        <is>
+          <t>Resources (Other)</t>
+        </is>
+      </c>
+    </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
@@ -22013,6 +22290,2025 @@
         <v>0</v>
       </c>
       <c r="BC2" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>33rd DAA, San Benito County Fair</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>139079</v>
+      </c>
+      <c r="C3" t="n">
+        <v>180000</v>
+      </c>
+      <c r="D3" t="n">
+        <v>6000</v>
+      </c>
+      <c r="E3" t="n">
+        <v>59057</v>
+      </c>
+      <c r="F3" t="n">
+        <v>15300</v>
+      </c>
+      <c r="G3" t="n">
+        <v>36920</v>
+      </c>
+      <c r="H3" t="n">
+        <v>12745</v>
+      </c>
+      <c r="I3" t="n">
+        <v>16654</v>
+      </c>
+      <c r="J3" t="n">
+        <v>0</v>
+      </c>
+      <c r="K3" t="n">
+        <v>0</v>
+      </c>
+      <c r="L3" t="n">
+        <v>0</v>
+      </c>
+      <c r="M3" t="n">
+        <v>40707</v>
+      </c>
+      <c r="N3" t="n">
+        <v>2931</v>
+      </c>
+      <c r="O3" t="n">
+        <v>139829</v>
+      </c>
+      <c r="P3" t="n">
+        <v>-23850</v>
+      </c>
+      <c r="Q3" t="n">
+        <v>18432</v>
+      </c>
+      <c r="R3" t="n">
+        <v>180497</v>
+      </c>
+      <c r="S3" t="n">
+        <v>192879</v>
+      </c>
+      <c r="T3" t="n">
+        <v>24547</v>
+      </c>
+      <c r="U3" t="n">
+        <v>17372</v>
+      </c>
+      <c r="V3" t="n">
+        <v>7519</v>
+      </c>
+      <c r="W3" t="n">
+        <v>0</v>
+      </c>
+      <c r="X3" t="n">
+        <v>22797</v>
+      </c>
+      <c r="Y3" t="n">
+        <v>23798</v>
+      </c>
+      <c r="Z3" t="n">
+        <v>16406</v>
+      </c>
+      <c r="AA3" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB3" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC3" t="n">
+        <v>30941</v>
+      </c>
+      <c r="AD3" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE3" t="n">
+        <v>3995</v>
+      </c>
+      <c r="AF3" t="n">
+        <v>3474</v>
+      </c>
+      <c r="AG3" t="n">
+        <v>-500</v>
+      </c>
+      <c r="AH3" t="n">
+        <v>31879</v>
+      </c>
+      <c r="AI3" t="n">
+        <v>0</v>
+      </c>
+      <c r="AJ3" t="n">
+        <v>0</v>
+      </c>
+      <c r="AK3" t="n">
+        <v>270803.16</v>
+      </c>
+      <c r="AL3" t="n">
+        <v>27170.58</v>
+      </c>
+      <c r="AM3" t="n">
+        <v>0</v>
+      </c>
+      <c r="AN3" t="n">
+        <v>61441.95</v>
+      </c>
+      <c r="AO3" t="n">
+        <v>1807671.35</v>
+      </c>
+      <c r="AP3" t="n">
+        <v>184692.02</v>
+      </c>
+      <c r="AQ3" t="n">
+        <v>0</v>
+      </c>
+      <c r="AR3" t="n">
+        <v>0</v>
+      </c>
+      <c r="AS3" t="n">
+        <v>14355.04</v>
+      </c>
+      <c r="AT3" t="n">
+        <v>4915.9</v>
+      </c>
+      <c r="AU3" t="n">
+        <v>0</v>
+      </c>
+      <c r="AV3" t="n">
+        <v>93790</v>
+      </c>
+      <c r="AW3" t="n">
+        <v>9155.41</v>
+      </c>
+      <c r="AX3" t="n">
+        <v>14372.72</v>
+      </c>
+      <c r="AY3" t="n">
+        <v>22371.6</v>
+      </c>
+      <c r="AZ3" t="n">
+        <v>2053805.32</v>
+      </c>
+      <c r="BA3" t="n">
+        <v>88200.32000000001</v>
+      </c>
+      <c r="BB3" t="n">
+        <v>14624</v>
+      </c>
+      <c r="BC3" t="n">
+        <v>36188.75</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>34th DAA, Modoc-Last Frontier Fair</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>32466</v>
+      </c>
+      <c r="C4" t="n">
+        <v>180000</v>
+      </c>
+      <c r="D4" t="n">
+        <v>0</v>
+      </c>
+      <c r="E4" t="n">
+        <v>11775</v>
+      </c>
+      <c r="F4" t="n">
+        <v>4398</v>
+      </c>
+      <c r="G4" t="n">
+        <v>6766</v>
+      </c>
+      <c r="H4" t="n">
+        <v>6216</v>
+      </c>
+      <c r="I4" t="n">
+        <v>20638</v>
+      </c>
+      <c r="J4" t="n">
+        <v>0</v>
+      </c>
+      <c r="K4" t="n">
+        <v>0</v>
+      </c>
+      <c r="L4" t="n">
+        <v>9670</v>
+      </c>
+      <c r="M4" t="n">
+        <v>4590</v>
+      </c>
+      <c r="N4" t="n">
+        <v>0</v>
+      </c>
+      <c r="O4" t="n">
+        <v>42402</v>
+      </c>
+      <c r="P4" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q4" t="n">
+        <v>5856</v>
+      </c>
+      <c r="R4" t="n">
+        <v>70503</v>
+      </c>
+      <c r="S4" t="n">
+        <v>91904</v>
+      </c>
+      <c r="T4" t="n">
+        <v>9575</v>
+      </c>
+      <c r="U4" t="n">
+        <v>5564</v>
+      </c>
+      <c r="V4" t="n">
+        <v>10050</v>
+      </c>
+      <c r="W4" t="n">
+        <v>0</v>
+      </c>
+      <c r="X4" t="n">
+        <v>13794</v>
+      </c>
+      <c r="Y4" t="n">
+        <v>10582</v>
+      </c>
+      <c r="Z4" t="n">
+        <v>22775</v>
+      </c>
+      <c r="AA4" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB4" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC4" t="n">
+        <v>31439</v>
+      </c>
+      <c r="AD4" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE4" t="n">
+        <v>0</v>
+      </c>
+      <c r="AF4" t="n">
+        <v>7628</v>
+      </c>
+      <c r="AG4" t="n">
+        <v>0</v>
+      </c>
+      <c r="AH4" t="n">
+        <v>4985</v>
+      </c>
+      <c r="AI4" t="n">
+        <v>0</v>
+      </c>
+      <c r="AJ4" t="n">
+        <v>0</v>
+      </c>
+      <c r="AK4" t="n">
+        <v>169956.27</v>
+      </c>
+      <c r="AL4" t="n">
+        <v>8606.17</v>
+      </c>
+      <c r="AM4" t="n">
+        <v>0</v>
+      </c>
+      <c r="AN4" t="n">
+        <v>600</v>
+      </c>
+      <c r="AO4" t="n">
+        <v>1153525.76</v>
+      </c>
+      <c r="AP4" t="n">
+        <v>63313.37</v>
+      </c>
+      <c r="AQ4" t="n">
+        <v>0</v>
+      </c>
+      <c r="AR4" t="n">
+        <v>0</v>
+      </c>
+      <c r="AS4" t="n">
+        <v>3414.3</v>
+      </c>
+      <c r="AT4" t="n">
+        <v>0</v>
+      </c>
+      <c r="AU4" t="n">
+        <v>0</v>
+      </c>
+      <c r="AV4" t="n">
+        <v>90000</v>
+      </c>
+      <c r="AW4" t="n">
+        <v>1275</v>
+      </c>
+      <c r="AX4" t="n">
+        <v>33208.53</v>
+      </c>
+      <c r="AY4" t="n">
+        <v>0</v>
+      </c>
+      <c r="AZ4" t="n">
+        <v>1217439.13</v>
+      </c>
+      <c r="BA4" t="n">
+        <v>45977.52</v>
+      </c>
+      <c r="BB4" t="n">
+        <v>4687.09</v>
+      </c>
+      <c r="BC4" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>41st DAA, Del Norte County Fair</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
+        <v>36513</v>
+      </c>
+      <c r="C5" t="n">
+        <v>180000</v>
+      </c>
+      <c r="D5" t="n">
+        <v>0</v>
+      </c>
+      <c r="E5" t="n">
+        <v>61683</v>
+      </c>
+      <c r="F5" t="n">
+        <v>0</v>
+      </c>
+      <c r="G5" t="n">
+        <v>62873</v>
+      </c>
+      <c r="H5" t="n">
+        <v>2330</v>
+      </c>
+      <c r="I5" t="n">
+        <v>1295</v>
+      </c>
+      <c r="J5" t="n">
+        <v>561</v>
+      </c>
+      <c r="K5" t="n">
+        <v>0</v>
+      </c>
+      <c r="L5" t="n">
+        <v>6254</v>
+      </c>
+      <c r="M5" t="n">
+        <v>3239</v>
+      </c>
+      <c r="N5" t="n">
+        <v>98778</v>
+      </c>
+      <c r="O5" t="n">
+        <v>-10869</v>
+      </c>
+      <c r="P5" t="n">
+        <v>14669</v>
+      </c>
+      <c r="Q5" t="n">
+        <v>169810</v>
+      </c>
+      <c r="R5" t="n">
+        <v>149284</v>
+      </c>
+      <c r="S5" t="n">
+        <v>11801</v>
+      </c>
+      <c r="T5" t="n">
+        <v>9140</v>
+      </c>
+      <c r="U5" t="n">
+        <v>4747</v>
+      </c>
+      <c r="V5" t="n">
+        <v>715</v>
+      </c>
+      <c r="W5" t="n">
+        <v>10167</v>
+      </c>
+      <c r="X5" t="n">
+        <v>15794</v>
+      </c>
+      <c r="Y5" t="n">
+        <v>407</v>
+      </c>
+      <c r="Z5" t="n">
+        <v>748</v>
+      </c>
+      <c r="AA5" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB5" t="n">
+        <v>46842</v>
+      </c>
+      <c r="AC5" t="n">
+        <v>12641</v>
+      </c>
+      <c r="AD5" t="n">
+        <v>4298</v>
+      </c>
+      <c r="AE5" t="n">
+        <v>-5492</v>
+      </c>
+      <c r="AF5" t="n">
+        <v>114</v>
+      </c>
+      <c r="AG5" t="n">
+        <v>5756</v>
+      </c>
+      <c r="AH5" t="n">
+        <v>0</v>
+      </c>
+      <c r="AI5" t="n">
+        <v>147817.72</v>
+      </c>
+      <c r="AJ5" t="n">
+        <v>260410.25</v>
+      </c>
+      <c r="AK5" t="n">
+        <v>845.05</v>
+      </c>
+      <c r="AL5" t="n">
+        <v>20352.53</v>
+      </c>
+      <c r="AM5" t="n">
+        <v>2003997.47</v>
+      </c>
+      <c r="AN5" t="n">
+        <v>190015.25</v>
+      </c>
+      <c r="AO5" t="n">
+        <v>0</v>
+      </c>
+      <c r="AP5" t="n">
+        <v>5965</v>
+      </c>
+      <c r="AQ5" t="n">
+        <v>9022</v>
+      </c>
+      <c r="AR5" t="n">
+        <v>1578.1</v>
+      </c>
+      <c r="AS5" t="n">
+        <v>0</v>
+      </c>
+      <c r="AT5" t="n">
+        <v>895</v>
+      </c>
+      <c r="AU5" t="n">
+        <v>13073.2</v>
+      </c>
+      <c r="AV5" t="n">
+        <v>3183.4</v>
+      </c>
+      <c r="AW5" t="n">
+        <v>20205268.11</v>
+      </c>
+      <c r="AX5" t="n">
+        <v>36996.19</v>
+      </c>
+      <c r="AY5" t="n">
+        <v>236864.7</v>
+      </c>
+      <c r="AZ5" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>44th DAA, Colusa County Fair</t>
+        </is>
+      </c>
+      <c r="B6" t="n">
+        <v>90944</v>
+      </c>
+      <c r="C6" t="n">
+        <v>180000</v>
+      </c>
+      <c r="D6" t="n">
+        <v>0</v>
+      </c>
+      <c r="E6" t="n">
+        <v>79267</v>
+      </c>
+      <c r="F6" t="n">
+        <v>6356</v>
+      </c>
+      <c r="G6" t="n">
+        <v>79908</v>
+      </c>
+      <c r="H6" t="n">
+        <v>3696</v>
+      </c>
+      <c r="I6" t="n">
+        <v>12621</v>
+      </c>
+      <c r="J6" t="n">
+        <v>1013</v>
+      </c>
+      <c r="K6" t="n">
+        <v>0</v>
+      </c>
+      <c r="L6" t="n">
+        <v>22452</v>
+      </c>
+      <c r="M6" t="n">
+        <v>34985</v>
+      </c>
+      <c r="N6" t="n">
+        <v>128299</v>
+      </c>
+      <c r="O6" t="n">
+        <v>64442</v>
+      </c>
+      <c r="P6" t="n">
+        <v>6021</v>
+      </c>
+      <c r="Q6" t="n">
+        <v>6296</v>
+      </c>
+      <c r="R6" t="n">
+        <v>156066</v>
+      </c>
+      <c r="S6" t="n">
+        <v>238331</v>
+      </c>
+      <c r="T6" t="n">
+        <v>23828</v>
+      </c>
+      <c r="U6" t="n">
+        <v>18487</v>
+      </c>
+      <c r="V6" t="n">
+        <v>1371</v>
+      </c>
+      <c r="W6" t="n">
+        <v>35</v>
+      </c>
+      <c r="X6" t="n">
+        <v>11739</v>
+      </c>
+      <c r="Y6" t="n">
+        <v>25711</v>
+      </c>
+      <c r="Z6" t="n">
+        <v>14767</v>
+      </c>
+      <c r="AA6" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB6" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC6" t="n">
+        <v>71404</v>
+      </c>
+      <c r="AD6" t="n">
+        <v>67786</v>
+      </c>
+      <c r="AE6" t="n">
+        <v>0</v>
+      </c>
+      <c r="AF6" t="n">
+        <v>6667</v>
+      </c>
+      <c r="AG6" t="n">
+        <v>-3</v>
+      </c>
+      <c r="AH6" t="n">
+        <v>0</v>
+      </c>
+      <c r="AI6" t="n">
+        <v>0</v>
+      </c>
+      <c r="AJ6" t="n">
+        <v>86661.10000000001</v>
+      </c>
+      <c r="AK6" t="n">
+        <v>204833.12</v>
+      </c>
+      <c r="AL6" t="n">
+        <v>17624.81</v>
+      </c>
+      <c r="AM6" t="n">
+        <v>10564.66</v>
+      </c>
+      <c r="AN6" t="n">
+        <v>3298.23</v>
+      </c>
+      <c r="AO6" t="n">
+        <v>961183.6899999999</v>
+      </c>
+      <c r="AP6" t="n">
+        <v>105897.85</v>
+      </c>
+      <c r="AQ6" t="n">
+        <v>0</v>
+      </c>
+      <c r="AR6" t="n">
+        <v>5831.52</v>
+      </c>
+      <c r="AS6" t="n">
+        <v>9679.280000000001</v>
+      </c>
+      <c r="AT6" t="n">
+        <v>1333.23</v>
+      </c>
+      <c r="AU6" t="n">
+        <v>0</v>
+      </c>
+      <c r="AV6" t="n">
+        <v>125665</v>
+      </c>
+      <c r="AW6" t="n">
+        <v>11750.68</v>
+      </c>
+      <c r="AX6" t="n">
+        <v>37210</v>
+      </c>
+      <c r="AY6" t="n">
+        <v>37824.78</v>
+      </c>
+      <c r="AZ6" t="n">
+        <v>1070379.77</v>
+      </c>
+      <c r="BA6" t="n">
+        <v>80111.02</v>
+      </c>
+      <c r="BB6" t="n">
+        <v>10278.18</v>
+      </c>
+      <c r="BC6" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>51st DAA, San Fernando Valley Fair</t>
+        </is>
+      </c>
+      <c r="B7" t="n">
+        <v>-527932</v>
+      </c>
+      <c r="C7" t="n">
+        <v>180000</v>
+      </c>
+      <c r="D7" t="n">
+        <v>0</v>
+      </c>
+      <c r="E7" t="n">
+        <v>66282</v>
+      </c>
+      <c r="F7" t="n">
+        <v>20725</v>
+      </c>
+      <c r="G7" t="n">
+        <v>45686</v>
+      </c>
+      <c r="H7" t="n">
+        <v>965</v>
+      </c>
+      <c r="I7" t="n">
+        <v>0</v>
+      </c>
+      <c r="J7" t="n">
+        <v>0</v>
+      </c>
+      <c r="K7" t="n">
+        <v>0</v>
+      </c>
+      <c r="L7" t="n">
+        <v>0</v>
+      </c>
+      <c r="M7" t="n">
+        <v>65035</v>
+      </c>
+      <c r="N7" t="n">
+        <v>132</v>
+      </c>
+      <c r="O7" t="n">
+        <v>0</v>
+      </c>
+      <c r="P7" t="n">
+        <v>9577</v>
+      </c>
+      <c r="Q7" t="n">
+        <v>131383</v>
+      </c>
+      <c r="R7" t="n">
+        <v>185637</v>
+      </c>
+      <c r="S7" t="n">
+        <v>8781</v>
+      </c>
+      <c r="T7" t="n">
+        <v>42113</v>
+      </c>
+      <c r="U7" t="n">
+        <v>33027</v>
+      </c>
+      <c r="V7" t="n">
+        <v>45786</v>
+      </c>
+      <c r="W7" t="n">
+        <v>0</v>
+      </c>
+      <c r="X7" t="n">
+        <v>1744</v>
+      </c>
+      <c r="Y7" t="n">
+        <v>38015</v>
+      </c>
+      <c r="Z7" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA7" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB7" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC7" t="n">
+        <v>98727</v>
+      </c>
+      <c r="AD7" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE7" t="n">
+        <v>1070</v>
+      </c>
+      <c r="AF7" t="n">
+        <v>-176363</v>
+      </c>
+      <c r="AG7" t="n">
+        <v>249</v>
+      </c>
+      <c r="AH7" t="n">
+        <v>0</v>
+      </c>
+      <c r="AI7" t="n">
+        <v>0</v>
+      </c>
+      <c r="AJ7" t="n">
+        <v>3000000</v>
+      </c>
+      <c r="AK7" t="n">
+        <v>-112686</v>
+      </c>
+      <c r="AL7" t="n">
+        <v>2884.75</v>
+      </c>
+      <c r="AM7" t="n">
+        <v>75</v>
+      </c>
+      <c r="AN7" t="n">
+        <v>0</v>
+      </c>
+      <c r="AO7" t="n">
+        <v>0</v>
+      </c>
+      <c r="AP7" t="n">
+        <v>35200.04</v>
+      </c>
+      <c r="AQ7" t="n">
+        <v>0</v>
+      </c>
+      <c r="AR7" t="n">
+        <v>0</v>
+      </c>
+      <c r="AS7" t="n">
+        <v>82117.13</v>
+      </c>
+      <c r="AT7" t="n">
+        <v>0</v>
+      </c>
+      <c r="AU7" t="n">
+        <v>633.25</v>
+      </c>
+      <c r="AV7" t="n">
+        <v>90100</v>
+      </c>
+      <c r="AW7" t="n">
+        <v>0</v>
+      </c>
+      <c r="AX7" t="n">
+        <v>0</v>
+      </c>
+      <c r="AY7" t="n">
+        <v>4355.71</v>
+      </c>
+      <c r="AZ7" t="n">
+        <v>35200.04</v>
+      </c>
+      <c r="BA7" t="n">
+        <v>-286932.5</v>
+      </c>
+      <c r="BB7" t="n">
+        <v>0</v>
+      </c>
+      <c r="BC7" t="n">
+        <v>3000000</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>52nd DAA, Sacto. County Fair</t>
+        </is>
+      </c>
+      <c r="B8" t="n">
+        <v>282969</v>
+      </c>
+      <c r="C8" t="n">
+        <v>180000</v>
+      </c>
+      <c r="D8" t="n">
+        <v>0</v>
+      </c>
+      <c r="E8" t="n">
+        <v>0</v>
+      </c>
+      <c r="F8" t="n">
+        <v>55737</v>
+      </c>
+      <c r="G8" t="n">
+        <v>91012</v>
+      </c>
+      <c r="H8" t="n">
+        <v>8707</v>
+      </c>
+      <c r="I8" t="n">
+        <v>0</v>
+      </c>
+      <c r="J8" t="n">
+        <v>0</v>
+      </c>
+      <c r="K8" t="n">
+        <v>0</v>
+      </c>
+      <c r="L8" t="n">
+        <v>2267</v>
+      </c>
+      <c r="M8" t="n">
+        <v>24998</v>
+      </c>
+      <c r="N8" t="n">
+        <v>0</v>
+      </c>
+      <c r="O8" t="n">
+        <v>189</v>
+      </c>
+      <c r="P8" t="n">
+        <v>754</v>
+      </c>
+      <c r="Q8" t="n">
+        <v>18485</v>
+      </c>
+      <c r="R8" t="n">
+        <v>193075</v>
+      </c>
+      <c r="S8" t="n">
+        <v>17253</v>
+      </c>
+      <c r="T8" t="n">
+        <v>38161</v>
+      </c>
+      <c r="U8" t="n">
+        <v>0</v>
+      </c>
+      <c r="V8" t="n">
+        <v>3319</v>
+      </c>
+      <c r="W8" t="n">
+        <v>0</v>
+      </c>
+      <c r="X8" t="n">
+        <v>13858</v>
+      </c>
+      <c r="Y8" t="n">
+        <v>34642</v>
+      </c>
+      <c r="Z8" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA8" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB8" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC8" t="n">
+        <v>24256</v>
+      </c>
+      <c r="AD8" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE8" t="n">
+        <v>0</v>
+      </c>
+      <c r="AF8" t="n">
+        <v>-1368</v>
+      </c>
+      <c r="AG8" t="n">
+        <v>0</v>
+      </c>
+      <c r="AH8" t="n">
+        <v>0</v>
+      </c>
+      <c r="AI8" t="n">
+        <v>0</v>
+      </c>
+      <c r="AJ8" t="n">
+        <v>38291</v>
+      </c>
+      <c r="AK8" t="n">
+        <v>441821.93</v>
+      </c>
+      <c r="AL8" t="n">
+        <v>3803.54</v>
+      </c>
+      <c r="AM8" t="n">
+        <v>0</v>
+      </c>
+      <c r="AN8" t="n">
+        <v>0</v>
+      </c>
+      <c r="AO8" t="n">
+        <v>20570</v>
+      </c>
+      <c r="AP8" t="n">
+        <v>10174.13</v>
+      </c>
+      <c r="AQ8" t="n">
+        <v>0</v>
+      </c>
+      <c r="AR8" t="n">
+        <v>0</v>
+      </c>
+      <c r="AS8" t="n">
+        <v>10789.28</v>
+      </c>
+      <c r="AT8" t="n">
+        <v>542.61</v>
+      </c>
+      <c r="AU8" t="n">
+        <v>0</v>
+      </c>
+      <c r="AV8" t="n">
+        <v>90000</v>
+      </c>
+      <c r="AW8" t="n">
+        <v>0</v>
+      </c>
+      <c r="AX8" t="n">
+        <v>0</v>
+      </c>
+      <c r="AY8" t="n">
+        <v>38271</v>
+      </c>
+      <c r="AZ8" t="n">
+        <v>30744.13</v>
+      </c>
+      <c r="BA8" t="n">
+        <v>341922.22</v>
+      </c>
+      <c r="BB8" t="n">
+        <v>2391.36</v>
+      </c>
+      <c r="BC8" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>54th DAA, Colorado River Country</t>
+        </is>
+      </c>
+      <c r="B9" t="n">
+        <v>-5850</v>
+      </c>
+      <c r="C9" t="n">
+        <v>180000</v>
+      </c>
+      <c r="D9" t="n">
+        <v>350</v>
+      </c>
+      <c r="E9" t="n">
+        <v>54812</v>
+      </c>
+      <c r="F9" t="n">
+        <v>0</v>
+      </c>
+      <c r="G9" t="n">
+        <v>52263</v>
+      </c>
+      <c r="H9" t="n">
+        <v>3828</v>
+      </c>
+      <c r="I9" t="n">
+        <v>0</v>
+      </c>
+      <c r="J9" t="n">
+        <v>0</v>
+      </c>
+      <c r="K9" t="n">
+        <v>0</v>
+      </c>
+      <c r="L9" t="n">
+        <v>8780</v>
+      </c>
+      <c r="M9" t="n">
+        <v>29743</v>
+      </c>
+      <c r="N9" t="n">
+        <v>0</v>
+      </c>
+      <c r="O9" t="n">
+        <v>81224</v>
+      </c>
+      <c r="P9" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q9" t="n">
+        <v>70</v>
+      </c>
+      <c r="R9" t="n">
+        <v>138106</v>
+      </c>
+      <c r="S9" t="n">
+        <v>137466</v>
+      </c>
+      <c r="T9" t="n">
+        <v>4981</v>
+      </c>
+      <c r="U9" t="n">
+        <v>17420</v>
+      </c>
+      <c r="V9" t="n">
+        <v>11568</v>
+      </c>
+      <c r="W9" t="n">
+        <v>16301</v>
+      </c>
+      <c r="X9" t="n">
+        <v>6282</v>
+      </c>
+      <c r="Y9" t="n">
+        <v>18920</v>
+      </c>
+      <c r="Z9" t="n">
+        <v>1580</v>
+      </c>
+      <c r="AA9" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB9" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC9" t="n">
+        <v>72939</v>
+      </c>
+      <c r="AD9" t="n">
+        <v>2048</v>
+      </c>
+      <c r="AE9" t="n">
+        <v>0</v>
+      </c>
+      <c r="AF9" t="n">
+        <v>-49928</v>
+      </c>
+      <c r="AG9" t="n">
+        <v>-210</v>
+      </c>
+      <c r="AH9" t="n">
+        <v>9970</v>
+      </c>
+      <c r="AI9" t="n">
+        <v>-108135</v>
+      </c>
+      <c r="AJ9" t="n">
+        <v>0</v>
+      </c>
+      <c r="AK9" t="n">
+        <v>7113.94</v>
+      </c>
+      <c r="AL9" t="n">
+        <v>2311.71</v>
+      </c>
+      <c r="AM9" t="n">
+        <v>4864.78</v>
+      </c>
+      <c r="AN9" t="n">
+        <v>61307.5</v>
+      </c>
+      <c r="AO9" t="n">
+        <v>1745603.12</v>
+      </c>
+      <c r="AP9" t="n">
+        <v>159220</v>
+      </c>
+      <c r="AQ9" t="n">
+        <v>0</v>
+      </c>
+      <c r="AR9" t="n">
+        <v>444</v>
+      </c>
+      <c r="AS9" t="n">
+        <v>31168.37</v>
+      </c>
+      <c r="AT9" t="n">
+        <v>875.17</v>
+      </c>
+      <c r="AU9" t="n">
+        <v>0</v>
+      </c>
+      <c r="AV9" t="n">
+        <v>35848</v>
+      </c>
+      <c r="AW9" t="n">
+        <v>18372.47</v>
+      </c>
+      <c r="AX9" t="n">
+        <v>17938.38</v>
+      </c>
+      <c r="AY9" t="n">
+        <v>0</v>
+      </c>
+      <c r="AZ9" t="n">
+        <v>1966130.62</v>
+      </c>
+      <c r="BA9" t="n">
+        <v>-90355.81</v>
+      </c>
+      <c r="BB9" t="n">
+        <v>0</v>
+      </c>
+      <c r="BC9" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>Cloverdale Citrus Fair</t>
+        </is>
+      </c>
+      <c r="B10" t="n">
+        <v>-49035</v>
+      </c>
+      <c r="C10" t="n">
+        <v>180000</v>
+      </c>
+      <c r="D10" t="n">
+        <v>16631</v>
+      </c>
+      <c r="E10" t="n">
+        <v>30443</v>
+      </c>
+      <c r="F10" t="n">
+        <v>5200</v>
+      </c>
+      <c r="G10" t="n">
+        <v>19426</v>
+      </c>
+      <c r="H10" t="n">
+        <v>3790</v>
+      </c>
+      <c r="I10" t="n">
+        <v>0</v>
+      </c>
+      <c r="J10" t="n">
+        <v>0</v>
+      </c>
+      <c r="K10" t="n">
+        <v>0</v>
+      </c>
+      <c r="L10" t="n">
+        <v>970</v>
+      </c>
+      <c r="M10" t="n">
+        <v>30840</v>
+      </c>
+      <c r="N10" t="n">
+        <v>77371</v>
+      </c>
+      <c r="O10" t="n">
+        <v>95780</v>
+      </c>
+      <c r="P10" t="n">
+        <v>39</v>
+      </c>
+      <c r="Q10" t="n">
+        <v>8087</v>
+      </c>
+      <c r="R10" t="n">
+        <v>101849</v>
+      </c>
+      <c r="S10" t="n">
+        <v>77178</v>
+      </c>
+      <c r="T10" t="n">
+        <v>12689</v>
+      </c>
+      <c r="U10" t="n">
+        <v>6058</v>
+      </c>
+      <c r="V10" t="n">
+        <v>5478</v>
+      </c>
+      <c r="W10" t="n">
+        <v>64243</v>
+      </c>
+      <c r="X10" t="n">
+        <v>11725</v>
+      </c>
+      <c r="Y10" t="n">
+        <v>2599</v>
+      </c>
+      <c r="Z10" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA10" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB10" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC10" t="n">
+        <v>29167</v>
+      </c>
+      <c r="AD10" t="n">
+        <v>8446</v>
+      </c>
+      <c r="AE10" t="n">
+        <v>5746</v>
+      </c>
+      <c r="AF10" t="n">
+        <v>2910</v>
+      </c>
+      <c r="AG10" t="n">
+        <v>-2</v>
+      </c>
+      <c r="AH10" t="n">
+        <v>2282</v>
+      </c>
+      <c r="AI10" t="n">
+        <v>0</v>
+      </c>
+      <c r="AJ10" t="n">
+        <v>0</v>
+      </c>
+      <c r="AK10" t="n">
+        <v>195728.76</v>
+      </c>
+      <c r="AL10" t="n">
+        <v>1611.91</v>
+      </c>
+      <c r="AM10" t="n">
+        <v>20425.63</v>
+      </c>
+      <c r="AN10" t="n">
+        <v>27233.35</v>
+      </c>
+      <c r="AO10" t="n">
+        <v>749234.72</v>
+      </c>
+      <c r="AP10" t="n">
+        <v>64233.46</v>
+      </c>
+      <c r="AQ10" t="n">
+        <v>0</v>
+      </c>
+      <c r="AR10" t="n">
+        <v>42</v>
+      </c>
+      <c r="AS10" t="n">
+        <v>884.0599999999999</v>
+      </c>
+      <c r="AT10" t="n">
+        <v>1492.29</v>
+      </c>
+      <c r="AU10" t="n">
+        <v>0</v>
+      </c>
+      <c r="AV10" t="n">
+        <v>114467</v>
+      </c>
+      <c r="AW10" t="n">
+        <v>6652</v>
+      </c>
+      <c r="AX10" t="n">
+        <v>3386.47</v>
+      </c>
+      <c r="AY10" t="n">
+        <v>0</v>
+      </c>
+      <c r="AZ10" t="n">
+        <v>840701.53</v>
+      </c>
+      <c r="BA10" t="n">
+        <v>89173.5</v>
+      </c>
+      <c r="BB10" t="n">
+        <v>1669</v>
+      </c>
+      <c r="BC10" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>Chowchilla- Madera County Fair</t>
+        </is>
+      </c>
+      <c r="B11" t="n">
+        <v>-21577</v>
+      </c>
+      <c r="C11" t="n">
+        <v>180000</v>
+      </c>
+      <c r="D11" t="n">
+        <v>0</v>
+      </c>
+      <c r="E11" t="n">
+        <v>51742</v>
+      </c>
+      <c r="F11" t="n">
+        <v>8212</v>
+      </c>
+      <c r="G11" t="n">
+        <v>39151</v>
+      </c>
+      <c r="H11" t="n">
+        <v>14889</v>
+      </c>
+      <c r="I11" t="n">
+        <v>0</v>
+      </c>
+      <c r="J11" t="n">
+        <v>0</v>
+      </c>
+      <c r="K11" t="n">
+        <v>0</v>
+      </c>
+      <c r="L11" t="n">
+        <v>7057</v>
+      </c>
+      <c r="M11" t="n">
+        <v>11873</v>
+      </c>
+      <c r="N11" t="n">
+        <v>73774</v>
+      </c>
+      <c r="O11" t="n">
+        <v>72312</v>
+      </c>
+      <c r="P11" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q11" t="n">
+        <v>12157</v>
+      </c>
+      <c r="R11" t="n">
+        <v>165491</v>
+      </c>
+      <c r="S11" t="n">
+        <v>164632</v>
+      </c>
+      <c r="T11" t="n">
+        <v>10874</v>
+      </c>
+      <c r="U11" t="n">
+        <v>15794</v>
+      </c>
+      <c r="V11" t="n">
+        <v>4217</v>
+      </c>
+      <c r="W11" t="n">
+        <v>17329</v>
+      </c>
+      <c r="X11" t="n">
+        <v>19229</v>
+      </c>
+      <c r="Y11" t="n">
+        <v>13878</v>
+      </c>
+      <c r="Z11" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA11" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB11" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC11" t="n">
+        <v>53111</v>
+      </c>
+      <c r="AD11" t="n">
+        <v>220</v>
+      </c>
+      <c r="AE11" t="n">
+        <v>0</v>
+      </c>
+      <c r="AF11" t="n">
+        <v>0</v>
+      </c>
+      <c r="AG11" t="n">
+        <v>0</v>
+      </c>
+      <c r="AH11" t="n">
+        <v>12784</v>
+      </c>
+      <c r="AI11" t="n">
+        <v>0</v>
+      </c>
+      <c r="AJ11" t="n">
+        <v>0</v>
+      </c>
+      <c r="AK11" t="n">
+        <v>199299.45</v>
+      </c>
+      <c r="AL11" t="n">
+        <v>11457.06</v>
+      </c>
+      <c r="AM11" t="n">
+        <v>45781.71</v>
+      </c>
+      <c r="AN11" t="n">
+        <v>90380.19</v>
+      </c>
+      <c r="AO11" t="n">
+        <v>3035666.9</v>
+      </c>
+      <c r="AP11" t="n">
+        <v>89744.13</v>
+      </c>
+      <c r="AQ11" t="n">
+        <v>0</v>
+      </c>
+      <c r="AR11" t="n">
+        <v>0</v>
+      </c>
+      <c r="AS11" t="n">
+        <v>8273.379999999999</v>
+      </c>
+      <c r="AT11" t="n">
+        <v>4592.73</v>
+      </c>
+      <c r="AU11" t="n">
+        <v>0</v>
+      </c>
+      <c r="AV11" t="n">
+        <v>337104.07</v>
+      </c>
+      <c r="AW11" t="n">
+        <v>0</v>
+      </c>
+      <c r="AX11" t="n">
+        <v>2416.86</v>
+      </c>
+      <c r="AY11" t="n">
+        <v>2024.96</v>
+      </c>
+      <c r="AZ11" t="n">
+        <v>3145791.22</v>
+      </c>
+      <c r="BA11" t="n">
+        <v>-27970.45</v>
+      </c>
+      <c r="BB11" t="n">
+        <v>96.67</v>
+      </c>
+      <c r="BC11" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>Mendocino County Fair</t>
+        </is>
+      </c>
+      <c r="B12" t="n">
+        <v>101768</v>
+      </c>
+      <c r="C12" t="n">
+        <v>180000</v>
+      </c>
+      <c r="D12" t="n">
+        <v>5472</v>
+      </c>
+      <c r="E12" t="n">
+        <v>54957</v>
+      </c>
+      <c r="F12" t="n">
+        <v>8325</v>
+      </c>
+      <c r="G12" t="n">
+        <v>40214</v>
+      </c>
+      <c r="H12" t="n">
+        <v>4502</v>
+      </c>
+      <c r="I12" t="n">
+        <v>1890</v>
+      </c>
+      <c r="J12" t="n">
+        <v>0</v>
+      </c>
+      <c r="K12" t="n">
+        <v>0</v>
+      </c>
+      <c r="L12" t="n">
+        <v>735</v>
+      </c>
+      <c r="M12" t="n">
+        <v>35852</v>
+      </c>
+      <c r="N12" t="n">
+        <v>0</v>
+      </c>
+      <c r="O12" t="n">
+        <v>31607</v>
+      </c>
+      <c r="P12" t="n">
+        <v>2310</v>
+      </c>
+      <c r="Q12" t="n">
+        <v>0</v>
+      </c>
+      <c r="R12" t="n">
+        <v>119069</v>
+      </c>
+      <c r="S12" t="n">
+        <v>114703</v>
+      </c>
+      <c r="T12" t="n">
+        <v>6974</v>
+      </c>
+      <c r="U12" t="n">
+        <v>8981</v>
+      </c>
+      <c r="V12" t="n">
+        <v>13750</v>
+      </c>
+      <c r="W12" t="n">
+        <v>438</v>
+      </c>
+      <c r="X12" t="n">
+        <v>30558</v>
+      </c>
+      <c r="Y12" t="n">
+        <v>15172</v>
+      </c>
+      <c r="Z12" t="n">
+        <v>200</v>
+      </c>
+      <c r="AA12" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB12" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC12" t="n">
+        <v>19925</v>
+      </c>
+      <c r="AD12" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE12" t="n">
+        <v>1453</v>
+      </c>
+      <c r="AF12" t="n">
+        <v>14363</v>
+      </c>
+      <c r="AG12" t="n">
+        <v>0</v>
+      </c>
+      <c r="AH12" t="n">
+        <v>15271</v>
+      </c>
+      <c r="AI12" t="n">
+        <v>0</v>
+      </c>
+      <c r="AJ12" t="n">
+        <v>0</v>
+      </c>
+      <c r="AK12" t="n">
+        <v>130491.38</v>
+      </c>
+      <c r="AL12" t="n">
+        <v>0</v>
+      </c>
+      <c r="AM12" t="n">
+        <v>0</v>
+      </c>
+      <c r="AN12" t="n">
+        <v>21634.74</v>
+      </c>
+      <c r="AO12" t="n">
+        <v>1974803.66</v>
+      </c>
+      <c r="AP12" t="n">
+        <v>52993.88</v>
+      </c>
+      <c r="AQ12" t="n">
+        <v>0</v>
+      </c>
+      <c r="AR12" t="n">
+        <v>0</v>
+      </c>
+      <c r="AS12" t="n">
+        <v>0</v>
+      </c>
+      <c r="AT12" t="n">
+        <v>0</v>
+      </c>
+      <c r="AU12" t="n">
+        <v>0</v>
+      </c>
+      <c r="AV12" t="n">
+        <v>0</v>
+      </c>
+      <c r="AW12" t="n">
+        <v>550</v>
+      </c>
+      <c r="AX12" t="n">
+        <v>14363.17</v>
+      </c>
+      <c r="AY12" t="n">
+        <v>0</v>
+      </c>
+      <c r="AZ12" t="n">
+        <v>2049432.28</v>
+      </c>
+      <c r="BA12" t="n">
+        <v>106773</v>
+      </c>
+      <c r="BB12" t="n">
+        <v>8805.16</v>
+      </c>
+      <c r="BC12" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>Inter-Mountain Fair of Shasta</t>
+        </is>
+      </c>
+      <c r="B13" t="n">
+        <v>17229</v>
+      </c>
+      <c r="C13" t="n">
+        <v>180000</v>
+      </c>
+      <c r="D13" t="n">
+        <v>0</v>
+      </c>
+      <c r="E13" t="n">
+        <v>46236</v>
+      </c>
+      <c r="F13" t="n">
+        <v>7855</v>
+      </c>
+      <c r="G13" t="n">
+        <v>54177</v>
+      </c>
+      <c r="H13" t="n">
+        <v>4795</v>
+      </c>
+      <c r="I13" t="n">
+        <v>1043</v>
+      </c>
+      <c r="J13" t="n">
+        <v>0</v>
+      </c>
+      <c r="K13" t="n">
+        <v>0</v>
+      </c>
+      <c r="L13" t="n">
+        <v>57770</v>
+      </c>
+      <c r="M13" t="n">
+        <v>15574</v>
+      </c>
+      <c r="N13" t="n">
+        <v>0</v>
+      </c>
+      <c r="O13" t="n">
+        <v>100355</v>
+      </c>
+      <c r="P13" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q13" t="n">
+        <v>0</v>
+      </c>
+      <c r="R13" t="n">
+        <v>166306</v>
+      </c>
+      <c r="S13" t="n">
+        <v>145510</v>
+      </c>
+      <c r="T13" t="n">
+        <v>13748</v>
+      </c>
+      <c r="U13" t="n">
+        <v>18177</v>
+      </c>
+      <c r="V13" t="n">
+        <v>9395</v>
+      </c>
+      <c r="W13" t="n">
+        <v>0</v>
+      </c>
+      <c r="X13" t="n">
+        <v>28074</v>
+      </c>
+      <c r="Y13" t="n">
+        <v>24535</v>
+      </c>
+      <c r="Z13" t="n">
+        <v>417</v>
+      </c>
+      <c r="AA13" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB13" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC13" t="n">
+        <v>54169</v>
+      </c>
+      <c r="AD13" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE13" t="n">
+        <v>2000</v>
+      </c>
+      <c r="AF13" t="n">
+        <v>-159</v>
+      </c>
+      <c r="AG13" t="n">
+        <v>0</v>
+      </c>
+      <c r="AH13" t="n">
+        <v>0</v>
+      </c>
+      <c r="AI13" t="n">
+        <v>0</v>
+      </c>
+      <c r="AJ13" t="n">
+        <v>0</v>
+      </c>
+      <c r="AK13" t="n">
+        <v>110574</v>
+      </c>
+      <c r="AL13" t="n">
+        <v>155</v>
+      </c>
+      <c r="AM13" t="n">
+        <v>0</v>
+      </c>
+      <c r="AN13" t="n">
+        <v>999</v>
+      </c>
+      <c r="AO13" t="n">
+        <v>2482573</v>
+      </c>
+      <c r="AP13" t="n">
+        <v>178727</v>
+      </c>
+      <c r="AQ13" t="n">
+        <v>0</v>
+      </c>
+      <c r="AR13" t="n">
+        <v>0</v>
+      </c>
+      <c r="AS13" t="n">
+        <v>0</v>
+      </c>
+      <c r="AT13" t="n">
+        <v>0</v>
+      </c>
+      <c r="AU13" t="n">
+        <v>0</v>
+      </c>
+      <c r="AV13" t="n">
+        <v>90000</v>
+      </c>
+      <c r="AW13" t="n">
+        <v>0</v>
+      </c>
+      <c r="AX13" t="n">
+        <v>0</v>
+      </c>
+      <c r="AY13" t="n">
+        <v>3857</v>
+      </c>
+      <c r="AZ13" t="n">
+        <v>2662299</v>
+      </c>
+      <c r="BA13" t="n">
+        <v>22862</v>
+      </c>
+      <c r="BB13" t="n">
+        <v>-5990</v>
+      </c>
+      <c r="BC13" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>Trinity County Fair</t>
+        </is>
+      </c>
+      <c r="B14" t="n">
+        <v>13169</v>
+      </c>
+      <c r="C14" t="n">
+        <v>180000</v>
+      </c>
+      <c r="D14" t="n">
+        <v>0</v>
+      </c>
+      <c r="E14" t="n">
+        <v>16279</v>
+      </c>
+      <c r="F14" t="n">
+        <v>6883</v>
+      </c>
+      <c r="G14" t="n">
+        <v>20108</v>
+      </c>
+      <c r="H14" t="n">
+        <v>8567</v>
+      </c>
+      <c r="I14" t="n">
+        <v>1685</v>
+      </c>
+      <c r="J14" t="n">
+        <v>0</v>
+      </c>
+      <c r="K14" t="n">
+        <v>0</v>
+      </c>
+      <c r="L14" t="n">
+        <v>34469</v>
+      </c>
+      <c r="M14" t="n">
+        <v>5448</v>
+      </c>
+      <c r="N14" t="n">
+        <v>2146</v>
+      </c>
+      <c r="O14" t="n">
+        <v>97100</v>
+      </c>
+      <c r="P14" t="n">
+        <v>415</v>
+      </c>
+      <c r="Q14" t="n">
+        <v>0</v>
+      </c>
+      <c r="R14" t="n">
+        <v>115093</v>
+      </c>
+      <c r="S14" t="n">
+        <v>153005</v>
+      </c>
+      <c r="T14" t="n">
+        <v>5538</v>
+      </c>
+      <c r="U14" t="n">
+        <v>6851</v>
+      </c>
+      <c r="V14" t="n">
+        <v>2808</v>
+      </c>
+      <c r="W14" t="n">
+        <v>0</v>
+      </c>
+      <c r="X14" t="n">
+        <v>7606</v>
+      </c>
+      <c r="Y14" t="n">
+        <v>17815</v>
+      </c>
+      <c r="Z14" t="n">
+        <v>2517</v>
+      </c>
+      <c r="AA14" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB14" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC14" t="n">
+        <v>32817</v>
+      </c>
+      <c r="AD14" t="n">
+        <v>1243</v>
+      </c>
+      <c r="AE14" t="n">
+        <v>3500</v>
+      </c>
+      <c r="AF14" t="n">
+        <v>0</v>
+      </c>
+      <c r="AG14" t="n">
+        <v>0</v>
+      </c>
+      <c r="AH14" t="n">
+        <v>0</v>
+      </c>
+      <c r="AI14" t="n">
+        <v>0</v>
+      </c>
+      <c r="AJ14" t="n">
+        <v>0</v>
+      </c>
+      <c r="AK14" t="n">
+        <v>22640.46</v>
+      </c>
+      <c r="AL14" t="n">
+        <v>32204</v>
+      </c>
+      <c r="AM14" t="n">
+        <v>1053.47</v>
+      </c>
+      <c r="AN14" t="n">
+        <v>0</v>
+      </c>
+      <c r="AO14" t="n">
+        <v>0</v>
+      </c>
+      <c r="AP14" t="n">
+        <v>40131.25</v>
+      </c>
+      <c r="AQ14" t="n">
+        <v>0</v>
+      </c>
+      <c r="AR14" t="n">
+        <v>0</v>
+      </c>
+      <c r="AS14" t="n">
+        <v>0</v>
+      </c>
+      <c r="AT14" t="n">
+        <v>0</v>
+      </c>
+      <c r="AU14" t="n">
+        <v>0</v>
+      </c>
+      <c r="AV14" t="n">
+        <v>3392.91</v>
+      </c>
+      <c r="AW14" t="n">
+        <v>200</v>
+      </c>
+      <c r="AX14" t="n">
+        <v>6127.34</v>
+      </c>
+      <c r="AY14" t="n">
+        <v>8769.719999999999</v>
+      </c>
+      <c r="AZ14" t="n">
+        <v>40131.25</v>
+      </c>
+      <c r="BA14" t="n">
+        <v>37477</v>
+      </c>
+      <c r="BB14" t="n">
+        <v>-69</v>
+      </c>
+      <c r="BC14" t="n">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Iterative edits to STOP reports and auto_to_csv
</commit_message>
<xml_diff>
--- a/Data/2001 STOP Summary.xlsx
+++ b/Data/2001 STOP Summary.xlsx
@@ -14833,7 +14833,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:S199"/>
+  <dimension ref="A1:P199"/>
   <sheetViews>
     <sheetView topLeftCell="A38" workbookViewId="0">
       <selection activeCell="A46" sqref="A46"/>
@@ -18101,7 +18101,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:Z199"/>
+  <dimension ref="A1:W199"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="2" ySplit="4" topLeftCell="C5" activePane="bottomRight" state="frozen"/>
@@ -22733,7 +22733,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:Y199"/>
+  <dimension ref="A1:V199"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="2" ySplit="4" topLeftCell="C29" activePane="bottomRight" state="frozen"/>
@@ -27172,7 +27172,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:O199"/>
+  <dimension ref="A1:L199"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="2" ySplit="4" topLeftCell="C32" activePane="bottomRight" state="frozen"/>
@@ -29740,7 +29740,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:L199"/>
+  <dimension ref="A1:J199"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C39" sqref="C39"/>
@@ -31690,7 +31690,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:L199"/>
+  <dimension ref="A1:J199"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="2" ySplit="4" topLeftCell="C5" activePane="bottomRight" state="frozen"/>

</xml_diff>

<commit_message>
Working on building feature table
</commit_message>
<xml_diff>
--- a/Data/2001 STOP Summary.xlsx
+++ b/Data/2001 STOP Summary.xlsx
@@ -6445,11 +6445,7 @@
       <c r="BC4" t="n">
         <v>0</v>
       </c>
-      <c r="BD4" t="inlineStr">
-        <is>
-          <t>* Reserve not reconciled</t>
-        </is>
-      </c>
+      <c r="BD4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -14833,7 +14829,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:P199"/>
+  <dimension ref="A1:O84"/>
   <sheetViews>
     <sheetView topLeftCell="A38" workbookViewId="0">
       <selection activeCell="A46" sqref="A46"/>
@@ -17938,130 +17934,9 @@
       <c r="N77" s="92" t="n"/>
       <c r="O77" s="92" t="n"/>
     </row>
-    <row r="78"/>
-    <row r="79"/>
-    <row r="80"/>
-    <row r="81"/>
-    <row r="82"/>
-    <row r="83"/>
     <row r="84" ht="12.75" customHeight="1">
       <c r="A84" s="34" t="n"/>
     </row>
-    <row r="85"/>
-    <row r="86"/>
-    <row r="87"/>
-    <row r="88"/>
-    <row r="89"/>
-    <row r="90"/>
-    <row r="91"/>
-    <row r="92"/>
-    <row r="93"/>
-    <row r="94"/>
-    <row r="95"/>
-    <row r="96"/>
-    <row r="97"/>
-    <row r="98"/>
-    <row r="99"/>
-    <row r="100"/>
-    <row r="101"/>
-    <row r="102"/>
-    <row r="103"/>
-    <row r="104"/>
-    <row r="105"/>
-    <row r="106"/>
-    <row r="107"/>
-    <row r="108"/>
-    <row r="109"/>
-    <row r="110"/>
-    <row r="111"/>
-    <row r="112"/>
-    <row r="113"/>
-    <row r="114"/>
-    <row r="115"/>
-    <row r="116"/>
-    <row r="117"/>
-    <row r="118"/>
-    <row r="119"/>
-    <row r="120"/>
-    <row r="121"/>
-    <row r="122"/>
-    <row r="123"/>
-    <row r="124"/>
-    <row r="125"/>
-    <row r="126"/>
-    <row r="127"/>
-    <row r="128"/>
-    <row r="129"/>
-    <row r="130"/>
-    <row r="131"/>
-    <row r="132"/>
-    <row r="133"/>
-    <row r="134"/>
-    <row r="135"/>
-    <row r="136"/>
-    <row r="137"/>
-    <row r="138"/>
-    <row r="139"/>
-    <row r="140"/>
-    <row r="141"/>
-    <row r="142"/>
-    <row r="143"/>
-    <row r="144"/>
-    <row r="145"/>
-    <row r="146"/>
-    <row r="147"/>
-    <row r="148"/>
-    <row r="149"/>
-    <row r="150"/>
-    <row r="151"/>
-    <row r="152"/>
-    <row r="153"/>
-    <row r="154"/>
-    <row r="155"/>
-    <row r="156"/>
-    <row r="157"/>
-    <row r="158"/>
-    <row r="159"/>
-    <row r="160"/>
-    <row r="161"/>
-    <row r="162"/>
-    <row r="163"/>
-    <row r="164"/>
-    <row r="165"/>
-    <row r="166"/>
-    <row r="167"/>
-    <row r="168"/>
-    <row r="169"/>
-    <row r="170"/>
-    <row r="171"/>
-    <row r="172"/>
-    <row r="173"/>
-    <row r="174"/>
-    <row r="175"/>
-    <row r="176"/>
-    <row r="177"/>
-    <row r="178"/>
-    <row r="179"/>
-    <row r="180"/>
-    <row r="181"/>
-    <row r="182"/>
-    <row r="183"/>
-    <row r="184"/>
-    <row r="185"/>
-    <row r="186"/>
-    <row r="187"/>
-    <row r="188"/>
-    <row r="189"/>
-    <row r="190"/>
-    <row r="191"/>
-    <row r="192"/>
-    <row r="193"/>
-    <row r="194"/>
-    <row r="195"/>
-    <row r="196"/>
-    <row r="197"/>
-    <row r="198"/>
-    <row r="199"/>
   </sheetData>
   <mergeCells count="15">
     <mergeCell ref="N2:N3"/>
@@ -18101,7 +17976,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:W199"/>
+  <dimension ref="A1:V84"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="2" ySplit="4" topLeftCell="C5" activePane="bottomRight" state="frozen"/>
@@ -22563,130 +22438,9 @@
       <c r="U77" s="92" t="n"/>
       <c r="V77" s="92" t="n"/>
     </row>
-    <row r="78"/>
-    <row r="79"/>
-    <row r="80"/>
-    <row r="81"/>
-    <row r="82"/>
-    <row r="83"/>
     <row r="84" ht="12.75" customHeight="1">
       <c r="A84" s="34" t="n"/>
     </row>
-    <row r="85"/>
-    <row r="86"/>
-    <row r="87"/>
-    <row r="88"/>
-    <row r="89"/>
-    <row r="90"/>
-    <row r="91"/>
-    <row r="92"/>
-    <row r="93"/>
-    <row r="94"/>
-    <row r="95"/>
-    <row r="96"/>
-    <row r="97"/>
-    <row r="98"/>
-    <row r="99"/>
-    <row r="100"/>
-    <row r="101"/>
-    <row r="102"/>
-    <row r="103"/>
-    <row r="104"/>
-    <row r="105"/>
-    <row r="106"/>
-    <row r="107"/>
-    <row r="108"/>
-    <row r="109"/>
-    <row r="110"/>
-    <row r="111"/>
-    <row r="112"/>
-    <row r="113"/>
-    <row r="114"/>
-    <row r="115"/>
-    <row r="116"/>
-    <row r="117"/>
-    <row r="118"/>
-    <row r="119"/>
-    <row r="120"/>
-    <row r="121"/>
-    <row r="122"/>
-    <row r="123"/>
-    <row r="124"/>
-    <row r="125"/>
-    <row r="126"/>
-    <row r="127"/>
-    <row r="128"/>
-    <row r="129"/>
-    <row r="130"/>
-    <row r="131"/>
-    <row r="132"/>
-    <row r="133"/>
-    <row r="134"/>
-    <row r="135"/>
-    <row r="136"/>
-    <row r="137"/>
-    <row r="138"/>
-    <row r="139"/>
-    <row r="140"/>
-    <row r="141"/>
-    <row r="142"/>
-    <row r="143"/>
-    <row r="144"/>
-    <row r="145"/>
-    <row r="146"/>
-    <row r="147"/>
-    <row r="148"/>
-    <row r="149"/>
-    <row r="150"/>
-    <row r="151"/>
-    <row r="152"/>
-    <row r="153"/>
-    <row r="154"/>
-    <row r="155"/>
-    <row r="156"/>
-    <row r="157"/>
-    <row r="158"/>
-    <row r="159"/>
-    <row r="160"/>
-    <row r="161"/>
-    <row r="162"/>
-    <row r="163"/>
-    <row r="164"/>
-    <row r="165"/>
-    <row r="166"/>
-    <row r="167"/>
-    <row r="168"/>
-    <row r="169"/>
-    <row r="170"/>
-    <row r="171"/>
-    <row r="172"/>
-    <row r="173"/>
-    <row r="174"/>
-    <row r="175"/>
-    <row r="176"/>
-    <row r="177"/>
-    <row r="178"/>
-    <row r="179"/>
-    <row r="180"/>
-    <row r="181"/>
-    <row r="182"/>
-    <row r="183"/>
-    <row r="184"/>
-    <row r="185"/>
-    <row r="186"/>
-    <row r="187"/>
-    <row r="188"/>
-    <row r="189"/>
-    <row r="190"/>
-    <row r="191"/>
-    <row r="192"/>
-    <row r="193"/>
-    <row r="194"/>
-    <row r="195"/>
-    <row r="196"/>
-    <row r="197"/>
-    <row r="198"/>
-    <row r="199"/>
   </sheetData>
   <mergeCells count="22">
     <mergeCell ref="S2:S3"/>
@@ -22733,7 +22487,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:V199"/>
+  <dimension ref="A1:U85"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="2" ySplit="4" topLeftCell="C29" activePane="bottomRight" state="frozen"/>
@@ -27004,129 +26758,9 @@
       </c>
       <c r="F78" s="57" t="n"/>
     </row>
-    <row r="79"/>
-    <row r="80"/>
-    <row r="81"/>
-    <row r="82"/>
-    <row r="83"/>
-    <row r="84"/>
     <row r="85">
       <c r="A85" s="33" t="n"/>
     </row>
-    <row r="86"/>
-    <row r="87"/>
-    <row r="88"/>
-    <row r="89"/>
-    <row r="90"/>
-    <row r="91"/>
-    <row r="92"/>
-    <row r="93"/>
-    <row r="94"/>
-    <row r="95"/>
-    <row r="96"/>
-    <row r="97"/>
-    <row r="98"/>
-    <row r="99"/>
-    <row r="100"/>
-    <row r="101"/>
-    <row r="102"/>
-    <row r="103"/>
-    <row r="104"/>
-    <row r="105"/>
-    <row r="106"/>
-    <row r="107"/>
-    <row r="108"/>
-    <row r="109"/>
-    <row r="110"/>
-    <row r="111"/>
-    <row r="112"/>
-    <row r="113"/>
-    <row r="114"/>
-    <row r="115"/>
-    <row r="116"/>
-    <row r="117"/>
-    <row r="118"/>
-    <row r="119"/>
-    <row r="120"/>
-    <row r="121"/>
-    <row r="122"/>
-    <row r="123"/>
-    <row r="124"/>
-    <row r="125"/>
-    <row r="126"/>
-    <row r="127"/>
-    <row r="128"/>
-    <row r="129"/>
-    <row r="130"/>
-    <row r="131"/>
-    <row r="132"/>
-    <row r="133"/>
-    <row r="134"/>
-    <row r="135"/>
-    <row r="136"/>
-    <row r="137"/>
-    <row r="138"/>
-    <row r="139"/>
-    <row r="140"/>
-    <row r="141"/>
-    <row r="142"/>
-    <row r="143"/>
-    <row r="144"/>
-    <row r="145"/>
-    <row r="146"/>
-    <row r="147"/>
-    <row r="148"/>
-    <row r="149"/>
-    <row r="150"/>
-    <row r="151"/>
-    <row r="152"/>
-    <row r="153"/>
-    <row r="154"/>
-    <row r="155"/>
-    <row r="156"/>
-    <row r="157"/>
-    <row r="158"/>
-    <row r="159"/>
-    <row r="160"/>
-    <row r="161"/>
-    <row r="162"/>
-    <row r="163"/>
-    <row r="164"/>
-    <row r="165"/>
-    <row r="166"/>
-    <row r="167"/>
-    <row r="168"/>
-    <row r="169"/>
-    <row r="170"/>
-    <row r="171"/>
-    <row r="172"/>
-    <row r="173"/>
-    <row r="174"/>
-    <row r="175"/>
-    <row r="176"/>
-    <row r="177"/>
-    <row r="178"/>
-    <row r="179"/>
-    <row r="180"/>
-    <row r="181"/>
-    <row r="182"/>
-    <row r="183"/>
-    <row r="184"/>
-    <row r="185"/>
-    <row r="186"/>
-    <row r="187"/>
-    <row r="188"/>
-    <row r="189"/>
-    <row r="190"/>
-    <row r="191"/>
-    <row r="192"/>
-    <row r="193"/>
-    <row r="194"/>
-    <row r="195"/>
-    <row r="196"/>
-    <row r="197"/>
-    <row r="198"/>
-    <row r="199"/>
   </sheetData>
   <mergeCells count="21">
     <mergeCell ref="S2:S3"/>
@@ -27172,7 +26806,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:L199"/>
+  <dimension ref="A1:K85"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="2" ySplit="4" topLeftCell="C32" activePane="bottomRight" state="frozen"/>
@@ -29583,128 +29217,9 @@
       <c r="J79" s="92" t="n"/>
       <c r="K79" s="92" t="n"/>
     </row>
-    <row r="80"/>
-    <row r="81"/>
-    <row r="82"/>
-    <row r="83"/>
-    <row r="84"/>
     <row r="85">
       <c r="A85" s="33" t="n"/>
     </row>
-    <row r="86"/>
-    <row r="87"/>
-    <row r="88"/>
-    <row r="89"/>
-    <row r="90"/>
-    <row r="91"/>
-    <row r="92"/>
-    <row r="93"/>
-    <row r="94"/>
-    <row r="95"/>
-    <row r="96"/>
-    <row r="97"/>
-    <row r="98"/>
-    <row r="99"/>
-    <row r="100"/>
-    <row r="101"/>
-    <row r="102"/>
-    <row r="103"/>
-    <row r="104"/>
-    <row r="105"/>
-    <row r="106"/>
-    <row r="107"/>
-    <row r="108"/>
-    <row r="109"/>
-    <row r="110"/>
-    <row r="111"/>
-    <row r="112"/>
-    <row r="113"/>
-    <row r="114"/>
-    <row r="115"/>
-    <row r="116"/>
-    <row r="117"/>
-    <row r="118"/>
-    <row r="119"/>
-    <row r="120"/>
-    <row r="121"/>
-    <row r="122"/>
-    <row r="123"/>
-    <row r="124"/>
-    <row r="125"/>
-    <row r="126"/>
-    <row r="127"/>
-    <row r="128"/>
-    <row r="129"/>
-    <row r="130"/>
-    <row r="131"/>
-    <row r="132"/>
-    <row r="133"/>
-    <row r="134"/>
-    <row r="135"/>
-    <row r="136"/>
-    <row r="137"/>
-    <row r="138"/>
-    <row r="139"/>
-    <row r="140"/>
-    <row r="141"/>
-    <row r="142"/>
-    <row r="143"/>
-    <row r="144"/>
-    <row r="145"/>
-    <row r="146"/>
-    <row r="147"/>
-    <row r="148"/>
-    <row r="149"/>
-    <row r="150"/>
-    <row r="151"/>
-    <row r="152"/>
-    <row r="153"/>
-    <row r="154"/>
-    <row r="155"/>
-    <row r="156"/>
-    <row r="157"/>
-    <row r="158"/>
-    <row r="159"/>
-    <row r="160"/>
-    <row r="161"/>
-    <row r="162"/>
-    <row r="163"/>
-    <row r="164"/>
-    <row r="165"/>
-    <row r="166"/>
-    <row r="167"/>
-    <row r="168"/>
-    <row r="169"/>
-    <row r="170"/>
-    <row r="171"/>
-    <row r="172"/>
-    <row r="173"/>
-    <row r="174"/>
-    <row r="175"/>
-    <row r="176"/>
-    <row r="177"/>
-    <row r="178"/>
-    <row r="179"/>
-    <row r="180"/>
-    <row r="181"/>
-    <row r="182"/>
-    <row r="183"/>
-    <row r="184"/>
-    <row r="185"/>
-    <row r="186"/>
-    <row r="187"/>
-    <row r="188"/>
-    <row r="189"/>
-    <row r="190"/>
-    <row r="191"/>
-    <row r="192"/>
-    <row r="193"/>
-    <row r="194"/>
-    <row r="195"/>
-    <row r="196"/>
-    <row r="197"/>
-    <row r="198"/>
-    <row r="199"/>
   </sheetData>
   <mergeCells count="11">
     <mergeCell ref="K2:K3"/>
@@ -29740,7 +29255,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J199"/>
+  <dimension ref="A1:H85"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C39" sqref="C39"/>
@@ -31529,7 +31044,6 @@
       <c r="G78" s="92" t="n"/>
       <c r="H78" s="92" t="n"/>
     </row>
-    <row r="79"/>
     <row r="80">
       <c r="A80" s="29" t="inlineStr">
         <is>
@@ -31537,127 +31051,9 @@
         </is>
       </c>
     </row>
-    <row r="81"/>
-    <row r="82"/>
-    <row r="83"/>
-    <row r="84"/>
     <row r="85">
       <c r="A85" s="33" t="n"/>
     </row>
-    <row r="86"/>
-    <row r="87"/>
-    <row r="88"/>
-    <row r="89"/>
-    <row r="90"/>
-    <row r="91"/>
-    <row r="92"/>
-    <row r="93"/>
-    <row r="94"/>
-    <row r="95"/>
-    <row r="96"/>
-    <row r="97"/>
-    <row r="98"/>
-    <row r="99"/>
-    <row r="100"/>
-    <row r="101"/>
-    <row r="102"/>
-    <row r="103"/>
-    <row r="104"/>
-    <row r="105"/>
-    <row r="106"/>
-    <row r="107"/>
-    <row r="108"/>
-    <row r="109"/>
-    <row r="110"/>
-    <row r="111"/>
-    <row r="112"/>
-    <row r="113"/>
-    <row r="114"/>
-    <row r="115"/>
-    <row r="116"/>
-    <row r="117"/>
-    <row r="118"/>
-    <row r="119"/>
-    <row r="120"/>
-    <row r="121"/>
-    <row r="122"/>
-    <row r="123"/>
-    <row r="124"/>
-    <row r="125"/>
-    <row r="126"/>
-    <row r="127"/>
-    <row r="128"/>
-    <row r="129"/>
-    <row r="130"/>
-    <row r="131"/>
-    <row r="132"/>
-    <row r="133"/>
-    <row r="134"/>
-    <row r="135"/>
-    <row r="136"/>
-    <row r="137"/>
-    <row r="138"/>
-    <row r="139"/>
-    <row r="140"/>
-    <row r="141"/>
-    <row r="142"/>
-    <row r="143"/>
-    <row r="144"/>
-    <row r="145"/>
-    <row r="146"/>
-    <row r="147"/>
-    <row r="148"/>
-    <row r="149"/>
-    <row r="150"/>
-    <row r="151"/>
-    <row r="152"/>
-    <row r="153"/>
-    <row r="154"/>
-    <row r="155"/>
-    <row r="156"/>
-    <row r="157"/>
-    <row r="158"/>
-    <row r="159"/>
-    <row r="160"/>
-    <row r="161"/>
-    <row r="162"/>
-    <row r="163"/>
-    <row r="164"/>
-    <row r="165"/>
-    <row r="166"/>
-    <row r="167"/>
-    <row r="168"/>
-    <row r="169"/>
-    <row r="170"/>
-    <row r="171"/>
-    <row r="172"/>
-    <row r="173"/>
-    <row r="174"/>
-    <row r="175"/>
-    <row r="176"/>
-    <row r="177"/>
-    <row r="178"/>
-    <row r="179"/>
-    <row r="180"/>
-    <row r="181"/>
-    <row r="182"/>
-    <row r="183"/>
-    <row r="184"/>
-    <row r="185"/>
-    <row r="186"/>
-    <row r="187"/>
-    <row r="188"/>
-    <row r="189"/>
-    <row r="190"/>
-    <row r="191"/>
-    <row r="192"/>
-    <row r="193"/>
-    <row r="194"/>
-    <row r="195"/>
-    <row r="196"/>
-    <row r="197"/>
-    <row r="198"/>
-    <row r="199"/>
   </sheetData>
   <mergeCells count="8">
     <mergeCell ref="A49:B50"/>
@@ -31690,7 +31086,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J199"/>
+  <dimension ref="A1:H88"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="2" ySplit="4" topLeftCell="C5" activePane="bottomRight" state="frozen"/>
@@ -33555,7 +32951,6 @@
       <c r="G81" s="92" t="n"/>
       <c r="H81" s="92" t="n"/>
     </row>
-    <row r="82"/>
     <row r="83">
       <c r="A83" s="29" t="inlineStr">
         <is>
@@ -33563,124 +32958,9 @@
         </is>
       </c>
     </row>
-    <row r="84"/>
-    <row r="85"/>
-    <row r="86"/>
-    <row r="87"/>
     <row r="88">
       <c r="A88" s="33" t="n"/>
     </row>
-    <row r="89"/>
-    <row r="90"/>
-    <row r="91"/>
-    <row r="92"/>
-    <row r="93"/>
-    <row r="94"/>
-    <row r="95"/>
-    <row r="96"/>
-    <row r="97"/>
-    <row r="98"/>
-    <row r="99"/>
-    <row r="100"/>
-    <row r="101"/>
-    <row r="102"/>
-    <row r="103"/>
-    <row r="104"/>
-    <row r="105"/>
-    <row r="106"/>
-    <row r="107"/>
-    <row r="108"/>
-    <row r="109"/>
-    <row r="110"/>
-    <row r="111"/>
-    <row r="112"/>
-    <row r="113"/>
-    <row r="114"/>
-    <row r="115"/>
-    <row r="116"/>
-    <row r="117"/>
-    <row r="118"/>
-    <row r="119"/>
-    <row r="120"/>
-    <row r="121"/>
-    <row r="122"/>
-    <row r="123"/>
-    <row r="124"/>
-    <row r="125"/>
-    <row r="126"/>
-    <row r="127"/>
-    <row r="128"/>
-    <row r="129"/>
-    <row r="130"/>
-    <row r="131"/>
-    <row r="132"/>
-    <row r="133"/>
-    <row r="134"/>
-    <row r="135"/>
-    <row r="136"/>
-    <row r="137"/>
-    <row r="138"/>
-    <row r="139"/>
-    <row r="140"/>
-    <row r="141"/>
-    <row r="142"/>
-    <row r="143"/>
-    <row r="144"/>
-    <row r="145"/>
-    <row r="146"/>
-    <row r="147"/>
-    <row r="148"/>
-    <row r="149"/>
-    <row r="150"/>
-    <row r="151"/>
-    <row r="152"/>
-    <row r="153"/>
-    <row r="154"/>
-    <row r="155"/>
-    <row r="156"/>
-    <row r="157"/>
-    <row r="158"/>
-    <row r="159"/>
-    <row r="160"/>
-    <row r="161"/>
-    <row r="162"/>
-    <row r="163"/>
-    <row r="164"/>
-    <row r="165"/>
-    <row r="166"/>
-    <row r="167"/>
-    <row r="168"/>
-    <row r="169"/>
-    <row r="170"/>
-    <row r="171"/>
-    <row r="172"/>
-    <row r="173"/>
-    <row r="174"/>
-    <row r="175"/>
-    <row r="176"/>
-    <row r="177"/>
-    <row r="178"/>
-    <row r="179"/>
-    <row r="180"/>
-    <row r="181"/>
-    <row r="182"/>
-    <row r="183"/>
-    <row r="184"/>
-    <row r="185"/>
-    <row r="186"/>
-    <row r="187"/>
-    <row r="188"/>
-    <row r="189"/>
-    <row r="190"/>
-    <row r="191"/>
-    <row r="192"/>
-    <row r="193"/>
-    <row r="194"/>
-    <row r="195"/>
-    <row r="196"/>
-    <row r="197"/>
-    <row r="198"/>
-    <row r="199"/>
   </sheetData>
   <mergeCells count="8">
     <mergeCell ref="A52:B53"/>
@@ -33713,7 +32993,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J199"/>
+  <dimension ref="A1:H94"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
       <pane xSplit="2" ySplit="3" topLeftCell="C52" activePane="bottomRight" state="frozen"/>
@@ -35252,121 +34532,12 @@
         </is>
       </c>
     </row>
-    <row r="89"/>
     <row r="90">
       <c r="E90" s="36" t="n"/>
     </row>
-    <row r="91"/>
-    <row r="92"/>
-    <row r="93"/>
     <row r="94">
       <c r="A94" s="33" t="n"/>
     </row>
-    <row r="95"/>
-    <row r="96"/>
-    <row r="97"/>
-    <row r="98"/>
-    <row r="99"/>
-    <row r="100"/>
-    <row r="101"/>
-    <row r="102"/>
-    <row r="103"/>
-    <row r="104"/>
-    <row r="105"/>
-    <row r="106"/>
-    <row r="107"/>
-    <row r="108"/>
-    <row r="109"/>
-    <row r="110"/>
-    <row r="111"/>
-    <row r="112"/>
-    <row r="113"/>
-    <row r="114"/>
-    <row r="115"/>
-    <row r="116"/>
-    <row r="117"/>
-    <row r="118"/>
-    <row r="119"/>
-    <row r="120"/>
-    <row r="121"/>
-    <row r="122"/>
-    <row r="123"/>
-    <row r="124"/>
-    <row r="125"/>
-    <row r="126"/>
-    <row r="127"/>
-    <row r="128"/>
-    <row r="129"/>
-    <row r="130"/>
-    <row r="131"/>
-    <row r="132"/>
-    <row r="133"/>
-    <row r="134"/>
-    <row r="135"/>
-    <row r="136"/>
-    <row r="137"/>
-    <row r="138"/>
-    <row r="139"/>
-    <row r="140"/>
-    <row r="141"/>
-    <row r="142"/>
-    <row r="143"/>
-    <row r="144"/>
-    <row r="145"/>
-    <row r="146"/>
-    <row r="147"/>
-    <row r="148"/>
-    <row r="149"/>
-    <row r="150"/>
-    <row r="151"/>
-    <row r="152"/>
-    <row r="153"/>
-    <row r="154"/>
-    <row r="155"/>
-    <row r="156"/>
-    <row r="157"/>
-    <row r="158"/>
-    <row r="159"/>
-    <row r="160"/>
-    <row r="161"/>
-    <row r="162"/>
-    <row r="163"/>
-    <row r="164"/>
-    <row r="165"/>
-    <row r="166"/>
-    <row r="167"/>
-    <row r="168"/>
-    <row r="169"/>
-    <row r="170"/>
-    <row r="171"/>
-    <row r="172"/>
-    <row r="173"/>
-    <row r="174"/>
-    <row r="175"/>
-    <row r="176"/>
-    <row r="177"/>
-    <row r="178"/>
-    <row r="179"/>
-    <row r="180"/>
-    <row r="181"/>
-    <row r="182"/>
-    <row r="183"/>
-    <row r="184"/>
-    <row r="185"/>
-    <row r="186"/>
-    <row r="187"/>
-    <row r="188"/>
-    <row r="189"/>
-    <row r="190"/>
-    <row r="191"/>
-    <row r="192"/>
-    <row r="193"/>
-    <row r="194"/>
-    <row r="195"/>
-    <row r="196"/>
-    <row r="197"/>
-    <row r="198"/>
-    <row r="199"/>
   </sheetData>
   <mergeCells count="7">
     <mergeCell ref="E2:E3"/>

</xml_diff>